<commit_message>
Modif Moap_to_level : traitement csv OK
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -9,11 +9,11 @@
   <sheets>
     <sheet name="MAP" sheetId="1" r:id="rId1"/>
     <sheet name="LEVEL" sheetId="2" r:id="rId2"/>
-    <sheet name="LEVEL 2" sheetId="3" r:id="rId3"/>
+    <sheet name="BoatsAttackGame" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">BoatsAttackGame!$A$1:$BS$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">LEVEL!$A:$V</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'LEVEL 2'!$A$1:$BS$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">MAP!$A:$AE</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -1279,10 +1279,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1610,7 +1610,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4634,7 +4634,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4662,85 +4662,85 @@
       <c r="I1" s="75"/>
       <c r="J1" s="75"/>
       <c r="K1" s="75"/>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="67" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="68" t="s">
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="67" t="s">
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="68" t="s">
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="67" t="s">
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="67"/>
-      <c r="AV1" s="68" t="s">
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="68"/>
+      <c r="AV1" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="68" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="BI1" s="68"/>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="67" t="s">
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="67"/>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="68"/>
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
       <c r="BS1" s="69"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5160,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="BS3" s="29">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6243,7 +6243,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="39">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C9" s="42">
         <v>10</v>
@@ -15700,6 +15700,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="X1:AC1"/>
+    <mergeCell ref="AD1:AI1"/>
+    <mergeCell ref="AP1:AU1"/>
     <mergeCell ref="AJ1:AO1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D2:E2"/>
@@ -15707,16 +15717,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="X1:AC1"/>
-    <mergeCell ref="AD1:AI1"/>
-    <mergeCell ref="AP1:AU1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Modif Moap_to_level : rename level.c.new => level.c
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1246,10 +1246,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1259,24 +1277,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="63" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2534,7 +2534,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2560,10 +2560,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="64" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2588,8 +2588,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2612,8 +2612,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="58" t="s">
+      <c r="A6" s="66"/>
+      <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2638,8 +2638,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2662,8 +2662,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="58" t="s">
+      <c r="A8" s="66"/>
+      <c r="B8" s="64" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2688,8 +2688,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2712,8 +2712,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
-      <c r="B10" s="58" t="s">
+      <c r="A10" s="66"/>
+      <c r="B10" s="64" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2738,8 +2738,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2762,7 +2762,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="56" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2920,7 +2920,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="56" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3104,7 +3104,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3288,7 +3288,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="56" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3472,7 +3472,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="64"/>
+      <c r="A39" s="58"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="59" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3682,7 +3682,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="63" t="s">
+      <c r="A47" s="56" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3840,7 +3840,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="64"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3866,7 +3866,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="59" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4050,7 +4050,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="63" t="s">
+      <c r="A61" s="56" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4208,7 +4208,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="64"/>
+      <c r="A67" s="58"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4234,7 +4234,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="63" t="s">
+      <c r="A68" s="56" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4392,7 +4392,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="64"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4418,7 +4418,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="56" t="s">
+      <c r="A75" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4576,7 +4576,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="66"/>
+      <c r="A81" s="60"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4603,23 +4603,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4633,8 +4633,8 @@
   </sheetPr>
   <dimension ref="A1:BS52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4774,13 +4774,13 @@
         <v>14</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="26" t="s">
         <v>13</v>
@@ -4792,13 +4792,13 @@
         <v>14</v>
       </c>
       <c r="T2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="V2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W2" s="26" t="s">
         <v>13</v>
@@ -4810,13 +4810,13 @@
         <v>14</v>
       </c>
       <c r="Z2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AB2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AC2" s="26" t="s">
         <v>13</v>
@@ -4828,13 +4828,13 @@
         <v>14</v>
       </c>
       <c r="AF2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AG2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AH2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AI2" s="26" t="s">
         <v>13</v>
@@ -4846,13 +4846,13 @@
         <v>14</v>
       </c>
       <c r="AL2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AN2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AO2" s="26" t="s">
         <v>13</v>
@@ -4864,13 +4864,13 @@
         <v>14</v>
       </c>
       <c r="AR2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AS2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AT2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AU2" s="26" t="s">
         <v>13</v>
@@ -4882,13 +4882,13 @@
         <v>14</v>
       </c>
       <c r="AX2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AY2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="AZ2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BA2" s="26" t="s">
         <v>13</v>
@@ -4900,13 +4900,13 @@
         <v>14</v>
       </c>
       <c r="BD2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="BE2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="BF2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BG2" s="26" t="s">
         <v>13</v>
@@ -4918,13 +4918,13 @@
         <v>14</v>
       </c>
       <c r="BJ2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="BK2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="BL2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BM2" s="26" t="s">
         <v>13</v>
@@ -4936,13 +4936,13 @@
         <v>14</v>
       </c>
       <c r="BP2" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="BQ2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="BR2" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BS2" s="27" t="s">
         <v>13</v>
@@ -5383,7 +5383,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="39">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" s="42">
         <v>10</v>
@@ -15700,11 +15700,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
@@ -15717,6 +15712,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise au point level 1 to 10
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1085,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1276,10 +1276,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1291,37 +1309,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1334,6 +1331,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2536,7 +2560,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="71" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2564,7 +2588,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2590,10 +2614,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="72" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2618,8 +2642,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2642,8 +2666,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
-      <c r="B6" s="66" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2668,8 +2692,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2692,8 +2716,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
-      <c r="B8" s="66" t="s">
+      <c r="A8" s="74"/>
+      <c r="B8" s="72" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2718,8 +2742,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="66"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2742,8 +2766,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
-      <c r="B10" s="66" t="s">
+      <c r="A10" s="74"/>
+      <c r="B10" s="72" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2768,8 +2792,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2792,7 +2816,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="64" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2950,7 +2974,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="72"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -2976,7 +3000,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="64" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3134,7 +3158,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3160,7 +3184,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="64" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3318,7 +3342,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="72"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3344,7 +3368,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="64" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3502,7 +3526,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="72"/>
+      <c r="A39" s="66"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3528,7 +3552,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="67" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3712,7 +3736,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="71" t="s">
+      <c r="A47" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3870,7 +3894,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="72"/>
+      <c r="A53" s="66"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3896,7 +3920,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="64" t="s">
+      <c r="A54" s="67" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4080,7 +4104,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="64" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4238,7 +4262,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="72"/>
+      <c r="A67" s="66"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4264,7 +4288,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="71" t="s">
+      <c r="A68" s="64" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4422,7 +4446,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="72"/>
+      <c r="A74" s="66"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4448,7 +4472,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="64" t="s">
+      <c r="A75" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4606,7 +4630,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="74"/>
+      <c r="A81" s="68"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4633,23 +4657,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4664,7 +4688,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4675,128 +4699,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="83" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="75" t="s">
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="76" t="s">
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="75" t="s">
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="76" t="s">
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="76"/>
-      <c r="AG1" s="76"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="76"/>
-      <c r="AJ1" s="75" t="s">
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="76" t="s">
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="76"/>
-      <c r="AR1" s="76"/>
-      <c r="AS1" s="76"/>
-      <c r="AT1" s="76"/>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="75" t="s">
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="77"/>
+      <c r="AT1" s="77"/>
+      <c r="AU1" s="77"/>
+      <c r="AV1" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="75"/>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="75"/>
-      <c r="BB1" s="76" t="s">
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="76"/>
-      <c r="BE1" s="76"/>
-      <c r="BF1" s="76"/>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="75" t="s">
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="77"/>
+      <c r="BG1" s="77"/>
+      <c r="BH1" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="BI1" s="75"/>
-      <c r="BJ1" s="75"/>
-      <c r="BK1" s="75"/>
-      <c r="BL1" s="75"/>
-      <c r="BM1" s="75"/>
-      <c r="BN1" s="76" t="s">
+      <c r="BI1" s="78"/>
+      <c r="BJ1" s="78"/>
+      <c r="BK1" s="78"/>
+      <c r="BL1" s="78"/>
+      <c r="BM1" s="78"/>
+      <c r="BN1" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" s="76"/>
-      <c r="BP1" s="76"/>
-      <c r="BQ1" s="76"/>
-      <c r="BR1" s="76"/>
-      <c r="BS1" s="77"/>
+      <c r="BO1" s="77"/>
+      <c r="BP1" s="77"/>
+      <c r="BQ1" s="77"/>
+      <c r="BR1" s="77"/>
+      <c r="BS1" s="83"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="79"/>
+      <c r="A2" s="76"/>
       <c r="B2" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82" t="s">
+      <c r="D2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82" t="s">
+      <c r="G2" s="81"/>
+      <c r="H2" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="82"/>
+      <c r="K2" s="81"/>
       <c r="L2" s="26" t="s">
         <v>29</v>
       </c>
@@ -4988,10 +5012,10 @@
       <c r="C3" s="37">
         <v>9</v>
       </c>
-      <c r="D3" s="40">
-        <v>0</v>
-      </c>
-      <c r="E3" s="28">
+      <c r="D3" s="91">
+        <v>0</v>
+      </c>
+      <c r="E3" s="89">
         <v>0</v>
       </c>
       <c r="F3" s="28">
@@ -5000,16 +5024,16 @@
       <c r="G3" s="28">
         <v>16</v>
       </c>
-      <c r="H3" s="28">
-        <v>0</v>
-      </c>
-      <c r="I3" s="28">
-        <v>0</v>
-      </c>
-      <c r="J3" s="28">
-        <v>0</v>
-      </c>
-      <c r="K3" s="37">
+      <c r="H3" s="89">
+        <v>0</v>
+      </c>
+      <c r="I3" s="89">
+        <v>0</v>
+      </c>
+      <c r="J3" s="89">
+        <v>0</v>
+      </c>
+      <c r="K3" s="90">
         <v>0</v>
       </c>
       <c r="L3" s="40">
@@ -5028,10 +5052,10 @@
         <v>0</v>
       </c>
       <c r="Q3" s="41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R3" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="28">
         <v>0</v>
@@ -5049,7 +5073,7 @@
         <v>5</v>
       </c>
       <c r="X3" s="40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="28">
         <v>0</v>
@@ -5067,7 +5091,7 @@
         <v>10</v>
       </c>
       <c r="AD3" s="40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="28">
         <v>0</v>
@@ -5085,7 +5109,7 @@
         <v>15</v>
       </c>
       <c r="AJ3" s="40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="28">
         <v>0</v>
@@ -5103,7 +5127,7 @@
         <v>20</v>
       </c>
       <c r="AP3" s="40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="28">
         <v>0</v>
@@ -5121,7 +5145,7 @@
         <v>25</v>
       </c>
       <c r="AV3" s="40">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AW3" s="28">
         <v>0</v>
@@ -5139,13 +5163,13 @@
         <v>30</v>
       </c>
       <c r="BB3" s="40">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BC3" s="28">
         <v>0</v>
       </c>
       <c r="BD3" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BE3" s="28">
         <v>0</v>
@@ -5157,13 +5181,13 @@
         <v>35</v>
       </c>
       <c r="BH3" s="40">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="BI3" s="28">
         <v>0</v>
       </c>
       <c r="BJ3" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BK3" s="28">
         <v>0</v>
@@ -5181,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="BP3" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BQ3" s="28">
         <v>0</v>
@@ -5204,7 +5228,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="42">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" s="30">
         <v>28</v>
@@ -5216,7 +5240,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="30">
         <v>28</v>
@@ -5243,168 +5267,168 @@
         <v>0</v>
       </c>
       <c r="Q4" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R4" s="39">
+        <v>0</v>
+      </c>
+      <c r="S4" s="30">
+        <v>0</v>
+      </c>
+      <c r="T4" s="30">
+        <v>0</v>
+      </c>
+      <c r="U4" s="30">
+        <v>10</v>
+      </c>
+      <c r="V4" s="30">
+        <v>0</v>
+      </c>
+      <c r="W4" s="30">
+        <v>5</v>
+      </c>
+      <c r="X4" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="43">
+        <v>10</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="30">
+        <v>10</v>
+      </c>
+      <c r="AG4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="30">
+        <v>30</v>
+      </c>
+      <c r="AJ4" s="42">
         <v>1</v>
       </c>
-      <c r="S4" s="30">
-        <v>0</v>
-      </c>
-      <c r="T4" s="30">
-        <v>10</v>
-      </c>
-      <c r="U4" s="30">
-        <v>0</v>
-      </c>
-      <c r="V4" s="30">
-        <v>0</v>
-      </c>
-      <c r="W4" s="30">
-        <v>5</v>
-      </c>
-      <c r="X4" s="42">
+      <c r="AK4" s="30">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="30">
+        <v>10</v>
+      </c>
+      <c r="AN4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="43">
+        <v>40</v>
+      </c>
+      <c r="AP4" s="30">
         <v>2</v>
       </c>
-      <c r="Y4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="43">
-        <v>10</v>
-      </c>
-      <c r="AD4" s="30">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AG4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="30">
-        <v>15</v>
-      </c>
-      <c r="AJ4" s="42">
-        <v>4</v>
-      </c>
-      <c r="AK4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AM4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="43">
+      <c r="AQ4" s="30">
+        <v>10</v>
+      </c>
+      <c r="AR4" s="30">
         <v>20</v>
       </c>
-      <c r="AP4" s="30">
-        <v>5</v>
-      </c>
-      <c r="AQ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="30">
-        <v>10</v>
-      </c>
       <c r="AS4" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT4" s="30">
         <v>0</v>
       </c>
       <c r="AU4" s="30">
-        <v>25</v>
-      </c>
-      <c r="AV4" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AY4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BA4" s="43">
-        <v>30</v>
-      </c>
-      <c r="BB4" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG4" s="30">
-        <v>35</v>
-      </c>
-      <c r="BH4" s="42">
-        <v>8</v>
-      </c>
-      <c r="BI4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="43">
+        <v>60</v>
+      </c>
+      <c r="AV4" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="86">
+        <v>60</v>
+      </c>
+      <c r="BB4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="85">
+        <v>60</v>
+      </c>
+      <c r="BH4" s="84">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="86">
         <v>40</v>
       </c>
-      <c r="BN4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS4" s="31">
+      <c r="BN4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS4" s="87">
         <v>45</v>
       </c>
     </row>
@@ -5418,22 +5442,22 @@
       <c r="C5" s="38">
         <v>9</v>
       </c>
-      <c r="D5" s="42">
-        <v>0</v>
-      </c>
-      <c r="E5" s="30">
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
-        <v>0</v>
-      </c>
-      <c r="I5" s="30">
+      <c r="D5" s="84">
+        <v>0</v>
+      </c>
+      <c r="E5" s="85">
+        <v>0</v>
+      </c>
+      <c r="F5" s="85">
+        <v>0</v>
+      </c>
+      <c r="G5" s="85">
+        <v>0</v>
+      </c>
+      <c r="H5" s="85">
+        <v>0</v>
+      </c>
+      <c r="I5" s="85">
         <v>0</v>
       </c>
       <c r="J5" s="30">
@@ -5458,7 +5482,7 @@
         <v>10</v>
       </c>
       <c r="Q5" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R5" s="39">
         <v>1</v>
@@ -5476,7 +5500,7 @@
         <v>10</v>
       </c>
       <c r="W5" s="30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X5" s="42">
         <v>2</v>
@@ -5494,10 +5518,10 @@
         <v>10</v>
       </c>
       <c r="AC5" s="43">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="30">
         <v>0</v>
@@ -5512,10 +5536,10 @@
         <v>10</v>
       </c>
       <c r="AI5" s="30">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AJ5" s="42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK5" s="30">
         <v>0</v>
@@ -5530,10 +5554,10 @@
         <v>10</v>
       </c>
       <c r="AO5" s="43">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="AP5" s="30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AQ5" s="30">
         <v>0</v>
@@ -5548,78 +5572,78 @@
         <v>10</v>
       </c>
       <c r="AU5" s="30">
-        <v>25</v>
-      </c>
-      <c r="AV5" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW5" s="30">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="30">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="30">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="30">
-        <v>10</v>
-      </c>
-      <c r="BA5" s="43">
-        <v>30</v>
-      </c>
-      <c r="BB5" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="30">
-        <v>35</v>
-      </c>
-      <c r="BH5" s="42">
-        <v>8</v>
-      </c>
-      <c r="BI5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM5" s="43">
-        <v>40</v>
-      </c>
-      <c r="BN5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR5" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS5" s="31">
+        <v>50</v>
+      </c>
+      <c r="AV5" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="86">
+        <v>60</v>
+      </c>
+      <c r="BB5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="85">
+        <v>60</v>
+      </c>
+      <c r="BH5" s="84">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="86">
+        <v>60</v>
+      </c>
+      <c r="BN5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS5" s="87">
         <v>45</v>
       </c>
     </row>
@@ -5633,10 +5657,10 @@
       <c r="C6" s="38">
         <v>9</v>
       </c>
-      <c r="D6" s="42">
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
+      <c r="D6" s="84">
+        <v>0</v>
+      </c>
+      <c r="E6" s="85">
         <v>0</v>
       </c>
       <c r="F6" s="30">
@@ -5645,10 +5669,10 @@
       <c r="G6" s="30">
         <v>16</v>
       </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
+      <c r="H6" s="85">
+        <v>0</v>
+      </c>
+      <c r="I6" s="85">
         <v>0</v>
       </c>
       <c r="J6" s="30">
@@ -5673,65 +5697,65 @@
         <v>0</v>
       </c>
       <c r="Q6" s="43">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R6" s="39">
+        <v>0</v>
+      </c>
+      <c r="S6" s="30">
+        <v>0</v>
+      </c>
+      <c r="T6" s="30">
+        <v>0</v>
+      </c>
+      <c r="U6" s="30">
+        <v>0</v>
+      </c>
+      <c r="V6" s="30">
+        <v>10</v>
+      </c>
+      <c r="W6" s="30">
+        <v>30</v>
+      </c>
+      <c r="X6" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="30">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="43">
+        <v>40</v>
+      </c>
+      <c r="AD6" s="30">
         <v>1</v>
       </c>
-      <c r="S6" s="30">
-        <v>0</v>
-      </c>
-      <c r="T6" s="30">
-        <v>0</v>
-      </c>
-      <c r="U6" s="30">
-        <v>0</v>
-      </c>
-      <c r="V6" s="30">
-        <v>10</v>
-      </c>
-      <c r="W6" s="30">
-        <v>5</v>
-      </c>
-      <c r="X6" s="42">
+      <c r="AE6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="30">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="30">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="30">
+        <v>60</v>
+      </c>
+      <c r="AJ6" s="42">
         <v>2</v>
       </c>
-      <c r="Y6" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="30">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="43">
-        <v>10</v>
-      </c>
-      <c r="AD6" s="30">
-        <v>3</v>
-      </c>
-      <c r="AE6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="30">
-        <v>10</v>
-      </c>
-      <c r="AI6" s="30">
-        <v>15</v>
-      </c>
-      <c r="AJ6" s="42">
-        <v>4</v>
-      </c>
       <c r="AK6" s="30">
         <v>0</v>
       </c>
@@ -5742,99 +5766,99 @@
         <v>0</v>
       </c>
       <c r="AN6" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO6" s="43">
-        <v>20</v>
-      </c>
-      <c r="AP6" s="30">
-        <v>5</v>
-      </c>
-      <c r="AQ6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="30">
-        <v>10</v>
-      </c>
-      <c r="AU6" s="30">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="85">
         <v>25</v>
       </c>
-      <c r="AV6" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="30">
-        <v>10</v>
-      </c>
-      <c r="AY6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="43">
+      <c r="AV6" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="86">
         <v>30</v>
       </c>
-      <c r="BB6" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG6" s="30">
+      <c r="BB6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="85">
         <v>35</v>
       </c>
-      <c r="BH6" s="42">
+      <c r="BH6" s="84">
         <v>8</v>
       </c>
-      <c r="BI6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM6" s="43">
+      <c r="BI6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="86">
         <v>40</v>
       </c>
-      <c r="BN6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR6" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS6" s="31">
+      <c r="BN6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR6" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS6" s="87">
         <v>45</v>
       </c>
     </row>
@@ -5848,10 +5872,10 @@
       <c r="C7" s="38">
         <v>8</v>
       </c>
-      <c r="D7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
+      <c r="D7" s="84">
+        <v>0</v>
+      </c>
+      <c r="E7" s="85">
         <v>0</v>
       </c>
       <c r="F7" s="30">
@@ -5861,10 +5885,10 @@
         <v>16</v>
       </c>
       <c r="H7" s="30">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I7" s="30">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J7" s="30">
         <v>2</v>
@@ -5888,65 +5912,65 @@
         <v>0</v>
       </c>
       <c r="Q7" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R7" s="39">
+        <v>0</v>
+      </c>
+      <c r="S7" s="30">
+        <v>0</v>
+      </c>
+      <c r="T7" s="30">
+        <v>0</v>
+      </c>
+      <c r="U7" s="30">
+        <v>0</v>
+      </c>
+      <c r="V7" s="30">
+        <v>10</v>
+      </c>
+      <c r="W7" s="30">
+        <v>5</v>
+      </c>
+      <c r="X7" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>10</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="43">
+        <v>10</v>
+      </c>
+      <c r="AD7" s="30">
         <v>1</v>
       </c>
-      <c r="S7" s="30">
-        <v>0</v>
-      </c>
-      <c r="T7" s="30">
-        <v>0</v>
-      </c>
-      <c r="U7" s="30">
-        <v>0</v>
-      </c>
-      <c r="V7" s="30">
-        <v>10</v>
-      </c>
-      <c r="W7" s="30">
-        <v>5</v>
-      </c>
-      <c r="X7" s="42">
+      <c r="AE7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="30">
+        <v>10</v>
+      </c>
+      <c r="AG7" s="30">
+        <v>10</v>
+      </c>
+      <c r="AH7" s="30">
+        <v>10</v>
+      </c>
+      <c r="AI7" s="30">
+        <v>30</v>
+      </c>
+      <c r="AJ7" s="42">
         <v>2</v>
       </c>
-      <c r="Y7" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="30">
-        <v>10</v>
-      </c>
-      <c r="AA7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="43">
-        <v>10</v>
-      </c>
-      <c r="AD7" s="30">
-        <v>3</v>
-      </c>
-      <c r="AE7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="30">
-        <v>10</v>
-      </c>
-      <c r="AI7" s="30">
-        <v>15</v>
-      </c>
-      <c r="AJ7" s="42">
-        <v>4</v>
-      </c>
       <c r="AK7" s="30">
         <v>0</v>
       </c>
@@ -5954,102 +5978,102 @@
         <v>10</v>
       </c>
       <c r="AM7" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AN7" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO7" s="43">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AP7" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="30">
         <v>0</v>
       </c>
       <c r="AR7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT7" s="30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AU7" s="30">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="AV7" s="42">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AW7" s="30">
         <v>0</v>
       </c>
       <c r="AX7" s="30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AY7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA7" s="43">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="BB7" s="30">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BC7" s="30">
         <v>0</v>
       </c>
       <c r="BD7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BF7" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG7" s="30">
-        <v>35</v>
-      </c>
-      <c r="BH7" s="42">
-        <v>8</v>
-      </c>
-      <c r="BI7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="43">
+        <v>70</v>
+      </c>
+      <c r="BH7" s="84">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="86">
         <v>40</v>
       </c>
-      <c r="BN7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR7" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS7" s="31">
+      <c r="BN7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR7" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS7" s="87">
         <v>45</v>
       </c>
     </row>
@@ -6064,10 +6088,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="42">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E8" s="30">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F8" s="30">
         <v>4</v>
@@ -6076,10 +6100,10 @@
         <v>16</v>
       </c>
       <c r="H8" s="30">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I8" s="30">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J8" s="30">
         <v>4</v>
@@ -6088,7 +6112,7 @@
         <v>16</v>
       </c>
       <c r="L8" s="42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M8" s="30">
         <v>0</v>
@@ -6103,10 +6127,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R8" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S8" s="30">
         <v>0</v>
@@ -6121,10 +6145,10 @@
         <v>10</v>
       </c>
       <c r="W8" s="30">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="X8" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y8" s="30">
         <v>0</v>
@@ -6136,135 +6160,135 @@
         <v>0</v>
       </c>
       <c r="AB8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC8" s="43">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AD8" s="30">
         <v>3</v>
       </c>
       <c r="AE8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF8" s="30">
         <v>0</v>
       </c>
       <c r="AG8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AH8" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="30">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="AJ8" s="42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL8" s="30">
         <v>10</v>
       </c>
       <c r="AM8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AN8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO8" s="43">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="AP8" s="30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AQ8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AR8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AS8" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AT8" s="30">
         <v>10</v>
       </c>
       <c r="AU8" s="30">
-        <v>25</v>
-      </c>
-      <c r="AV8" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW8" s="30">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="30">
-        <v>10</v>
-      </c>
-      <c r="AY8" s="30">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="43">
+        <v>70</v>
+      </c>
+      <c r="AV8" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="86">
         <v>30</v>
       </c>
-      <c r="BB8" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="30">
+      <c r="BB8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="85">
         <v>35</v>
       </c>
-      <c r="BH8" s="42">
-        <v>8</v>
-      </c>
-      <c r="BI8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="43">
+      <c r="BH8" s="84">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="86">
         <v>40</v>
       </c>
-      <c r="BN8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR8" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS8" s="31">
+      <c r="BN8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR8" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS8" s="87">
         <v>45</v>
       </c>
     </row>
@@ -6278,10 +6302,10 @@
       <c r="C9" s="38">
         <v>13</v>
       </c>
-      <c r="D9" s="42">
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
+      <c r="D9" s="84">
+        <v>0</v>
+      </c>
+      <c r="E9" s="85">
         <v>0</v>
       </c>
       <c r="F9" s="30">
@@ -6290,10 +6314,10 @@
       <c r="G9" s="30">
         <v>16</v>
       </c>
-      <c r="H9" s="30">
-        <v>0</v>
-      </c>
-      <c r="I9" s="30">
+      <c r="H9" s="85">
+        <v>0</v>
+      </c>
+      <c r="I9" s="85">
         <v>0</v>
       </c>
       <c r="J9" s="30">
@@ -6303,43 +6327,43 @@
         <v>16</v>
       </c>
       <c r="L9" s="42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M9" s="30">
         <v>0</v>
       </c>
       <c r="N9" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O9" s="30">
         <v>0</v>
       </c>
       <c r="P9" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R9" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S9" s="30">
         <v>0</v>
       </c>
       <c r="T9" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U9" s="30">
         <v>0</v>
       </c>
       <c r="V9" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W9" s="30">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="X9" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y9" s="30">
         <v>0</v>
@@ -6351,19 +6375,19 @@
         <v>0</v>
       </c>
       <c r="AB9" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC9" s="43">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AD9" s="30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE9" s="30">
         <v>0</v>
       </c>
       <c r="AF9" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG9" s="30">
         <v>0</v>
@@ -6372,114 +6396,114 @@
         <v>10</v>
       </c>
       <c r="AI9" s="30">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="AJ9" s="42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AK9" s="30">
         <v>0</v>
       </c>
       <c r="AL9" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AM9" s="30">
         <v>0</v>
       </c>
       <c r="AN9" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO9" s="43">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="AP9" s="30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AQ9" s="30">
         <v>0</v>
       </c>
       <c r="AR9" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS9" s="30">
         <v>0</v>
       </c>
       <c r="AT9" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AU9" s="30">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="AV9" s="42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AW9" s="30">
         <v>0</v>
       </c>
       <c r="AX9" s="30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AY9" s="30">
         <v>0</v>
       </c>
       <c r="AZ9" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA9" s="43">
-        <v>30</v>
-      </c>
-      <c r="BB9" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="30">
+        <v>120</v>
+      </c>
+      <c r="BB9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="85">
         <v>35</v>
       </c>
-      <c r="BH9" s="42">
+      <c r="BH9" s="84">
         <v>8</v>
       </c>
-      <c r="BI9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM9" s="43">
+      <c r="BI9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="86">
         <v>40</v>
       </c>
-      <c r="BN9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR9" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS9" s="31">
+      <c r="BN9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR9" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS9" s="87">
         <v>45</v>
       </c>
     </row>
@@ -6494,31 +6518,31 @@
         <v>7</v>
       </c>
       <c r="D10" s="42">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E10" s="30">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F10" s="30">
         <v>2</v>
       </c>
       <c r="G10" s="30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="30">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I10" s="30">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
-        <v>0</v>
-      </c>
-      <c r="K10" s="38">
+        <v>28</v>
+      </c>
+      <c r="J10" s="85">
+        <v>0</v>
+      </c>
+      <c r="K10" s="88">
         <v>0</v>
       </c>
       <c r="L10" s="42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10" s="30">
         <v>0</v>
@@ -6533,10 +6557,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R10" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S10" s="30">
         <v>0</v>
@@ -6551,46 +6575,46 @@
         <v>0</v>
       </c>
       <c r="W10" s="30">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="X10" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y10" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z10" s="30">
         <v>10</v>
       </c>
       <c r="AA10" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB10" s="30">
         <v>0</v>
       </c>
       <c r="AC10" s="43">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AD10" s="30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE10" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AF10" s="30">
         <v>10</v>
       </c>
       <c r="AG10" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AH10" s="30">
         <v>0</v>
       </c>
       <c r="AI10" s="30">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="AJ10" s="42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AK10" s="30">
         <v>0</v>
@@ -6605,96 +6629,96 @@
         <v>0</v>
       </c>
       <c r="AO10" s="43">
-        <v>20</v>
-      </c>
-      <c r="AP10" s="30">
-        <v>5</v>
-      </c>
-      <c r="AQ10" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="30">
-        <v>10</v>
-      </c>
-      <c r="AS10" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="30">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="30">
+        <v>90</v>
+      </c>
+      <c r="AP10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="85">
         <v>25</v>
       </c>
-      <c r="AV10" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW10" s="30">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="30">
-        <v>10</v>
-      </c>
-      <c r="AY10" s="30">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="43">
+      <c r="AV10" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="86">
         <v>30</v>
       </c>
-      <c r="BB10" s="30">
-        <v>7</v>
-      </c>
-      <c r="BC10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG10" s="30">
+      <c r="BB10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="85">
         <v>35</v>
       </c>
-      <c r="BH10" s="42">
-        <v>8</v>
-      </c>
-      <c r="BI10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM10" s="43">
+      <c r="BH10" s="84">
+        <v>0</v>
+      </c>
+      <c r="BI10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="86">
         <v>40</v>
       </c>
-      <c r="BN10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR10" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS10" s="31">
+      <c r="BN10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR10" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS10" s="87">
         <v>45</v>
       </c>
     </row>
@@ -6708,10 +6732,10 @@
       <c r="C11" s="38">
         <v>9</v>
       </c>
-      <c r="D11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30">
+      <c r="D11" s="84">
+        <v>0</v>
+      </c>
+      <c r="E11" s="85">
         <v>0</v>
       </c>
       <c r="F11" s="30">
@@ -6720,10 +6744,10 @@
       <c r="G11" s="30">
         <v>15</v>
       </c>
-      <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="30">
+      <c r="H11" s="85">
+        <v>0</v>
+      </c>
+      <c r="I11" s="85">
         <v>0</v>
       </c>
       <c r="J11" s="30">
@@ -6733,7 +6757,7 @@
         <v>16</v>
       </c>
       <c r="L11" s="42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M11" s="30">
         <v>0</v>
@@ -6748,10 +6772,10 @@
         <v>0</v>
       </c>
       <c r="Q11" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R11" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S11" s="30">
         <v>0</v>
@@ -6766,10 +6790,10 @@
         <v>10</v>
       </c>
       <c r="W11" s="30">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="X11" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="30">
         <v>0</v>
@@ -6781,19 +6805,19 @@
         <v>0</v>
       </c>
       <c r="AB11" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC11" s="43">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AD11" s="30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE11" s="30">
         <v>0</v>
       </c>
       <c r="AF11" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG11" s="30">
         <v>0</v>
@@ -6802,61 +6826,61 @@
         <v>10</v>
       </c>
       <c r="AI11" s="30">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="AJ11" s="42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AK11" s="30">
         <v>0</v>
       </c>
       <c r="AL11" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AM11" s="30">
         <v>0</v>
       </c>
       <c r="AN11" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO11" s="43">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="AP11" s="30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AQ11" s="30">
         <v>0</v>
       </c>
       <c r="AR11" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS11" s="30">
         <v>0</v>
       </c>
       <c r="AT11" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AU11" s="30">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="AV11" s="42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AW11" s="30">
         <v>0</v>
       </c>
       <c r="AX11" s="30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AY11" s="30">
         <v>0</v>
       </c>
       <c r="AZ11" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA11" s="43">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="BB11" s="30">
         <v>7</v>
@@ -6963,7 +6987,7 @@
         <v>5</v>
       </c>
       <c r="Q12" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R12" s="39">
         <v>1</v>
@@ -6981,7 +7005,7 @@
         <v>5</v>
       </c>
       <c r="W12" s="30">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X12" s="42">
         <v>2</v>
@@ -6999,13 +7023,13 @@
         <v>5</v>
       </c>
       <c r="AC12" s="43">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="AD12" s="30">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AE12" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="30">
         <v>5</v>
@@ -7014,117 +7038,117 @@
         <v>5</v>
       </c>
       <c r="AH12" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI12" s="30">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="AJ12" s="42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AK12" s="30">
         <v>5</v>
       </c>
       <c r="AL12" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AM12" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="30">
         <v>5</v>
       </c>
       <c r="AO12" s="43">
-        <v>20</v>
-      </c>
-      <c r="AP12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AQ12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AR12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AS12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AT12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AU12" s="30">
+        <v>80</v>
+      </c>
+      <c r="AP12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="85">
         <v>25</v>
       </c>
-      <c r="AV12" s="42">
-        <v>6</v>
-      </c>
-      <c r="AW12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AX12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AY12" s="30">
-        <v>5</v>
-      </c>
-      <c r="AZ12" s="30">
-        <v>5</v>
-      </c>
-      <c r="BA12" s="43">
+      <c r="AV12" s="84">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="85">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BA12" s="86">
         <v>30</v>
       </c>
-      <c r="BB12" s="30">
+      <c r="BB12" s="85">
         <v>7</v>
       </c>
-      <c r="BC12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BG12" s="30">
+      <c r="BC12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BD12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BE12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BF12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BG12" s="85">
         <v>35</v>
       </c>
-      <c r="BH12" s="42">
+      <c r="BH12" s="84">
         <v>8</v>
       </c>
-      <c r="BI12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BK12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BM12" s="43">
+      <c r="BI12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BJ12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BK12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BM12" s="86">
         <v>40</v>
       </c>
-      <c r="BN12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BR12" s="30">
-        <v>0</v>
-      </c>
-      <c r="BS12" s="31">
+      <c r="BN12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BP12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BR12" s="85">
+        <v>0</v>
+      </c>
+      <c r="BS12" s="87">
         <v>45</v>
       </c>
     </row>
@@ -15730,6 +15754,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
@@ -15743,10 +15771,6 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Level 11 -> 19
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1085,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1270,34 +1270,55 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1307,6 +1328,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1334,30 +1373,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1664,7 +1679,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1675,75 +1690,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
+      <c r="B1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
     </row>
     <row r="2" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="62">
+      <c r="B2" s="75">
         <v>30</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
     </row>
     <row r="3" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+      <c r="A3" s="75">
         <v>19</v>
       </c>
       <c r="B3" s="3">
@@ -1838,7 +1853,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1873,7 +1888,7 @@
       <c r="AE4" s="2"/>
     </row>
     <row r="5" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="75"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1908,7 +1923,7 @@
       <c r="AE5" s="2"/>
     </row>
     <row r="6" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="75"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1943,7 +1958,7 @@
       <c r="AE6" s="2"/>
     </row>
     <row r="7" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -1978,7 +1993,7 @@
       <c r="AE7" s="2"/>
     </row>
     <row r="8" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -2013,7 +2028,7 @@
       <c r="AE8" s="2"/>
     </row>
     <row r="9" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -2048,7 +2063,7 @@
       <c r="AE9" s="2"/>
     </row>
     <row r="10" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -2083,7 +2098,7 @@
       <c r="AE10" s="2"/>
     </row>
     <row r="11" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="2">
         <v>8</v>
       </c>
@@ -2118,7 +2133,7 @@
       <c r="AE11" s="2"/>
     </row>
     <row r="12" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -2153,7 +2168,7 @@
       <c r="AE12" s="2"/>
     </row>
     <row r="13" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="75"/>
       <c r="B13" s="2">
         <v>10</v>
       </c>
@@ -2188,7 +2203,7 @@
       <c r="AE13" s="2"/>
     </row>
     <row r="14" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -2223,7 +2238,7 @@
       <c r="AE14" s="2"/>
     </row>
     <row r="15" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="2">
         <v>12</v>
       </c>
@@ -2258,7 +2273,7 @@
       <c r="AE15" s="2"/>
     </row>
     <row r="16" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="2">
         <v>13</v>
       </c>
@@ -2293,7 +2308,7 @@
       <c r="AE16" s="2"/>
     </row>
     <row r="17" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="2">
         <v>14</v>
       </c>
@@ -2328,7 +2343,7 @@
       <c r="AE17" s="2"/>
     </row>
     <row r="18" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="2">
         <v>15</v>
       </c>
@@ -2363,7 +2378,7 @@
       <c r="AE18" s="2"/>
     </row>
     <row r="19" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -2398,7 +2413,7 @@
       <c r="AE19" s="2"/>
     </row>
     <row r="20" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="75"/>
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -2433,7 +2448,7 @@
       <c r="AE20" s="2"/>
     </row>
     <row r="21" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -2494,10 +2509,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="83"/>
       <c r="C1" s="6">
         <v>1</v>
       </c>
@@ -2560,7 +2575,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="86" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2588,7 +2603,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="71"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2614,10 +2629,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2642,8 +2657,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2666,8 +2681,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
-      <c r="B6" s="72" t="s">
+      <c r="A6" s="81"/>
+      <c r="B6" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2692,8 +2707,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
-      <c r="B7" s="72"/>
+      <c r="A7" s="81"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2716,8 +2731,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="72" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="79" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2742,8 +2757,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2766,8 +2781,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="72" t="s">
+      <c r="A10" s="81"/>
+      <c r="B10" s="79" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2792,8 +2807,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="73"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2816,7 +2831,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="84" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2844,7 +2859,7 @@
       <c r="V12" s="21"/>
     </row>
     <row r="13" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="22" t="s">
         <v>12</v>
       </c>
@@ -2870,7 +2885,7 @@
       <c r="V13" s="14"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +2911,7 @@
       <c r="V14" s="14"/>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="22" t="s">
         <v>14</v>
       </c>
@@ -2922,7 +2937,7 @@
       <c r="V15" s="14"/>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="22" t="s">
         <v>15</v>
       </c>
@@ -2948,7 +2963,7 @@
       <c r="V16" s="14"/>
     </row>
     <row r="17" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="22" t="s">
         <v>16</v>
       </c>
@@ -2974,7 +2989,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="85"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3000,7 +3015,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="84" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3028,7 +3043,7 @@
       <c r="V19" s="21"/>
     </row>
     <row r="20" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="65"/>
+      <c r="A20" s="78"/>
       <c r="B20" s="22" t="s">
         <v>12</v>
       </c>
@@ -3054,7 +3069,7 @@
       <c r="V20" s="14"/>
     </row>
     <row r="21" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="22" t="s">
         <v>13</v>
       </c>
@@ -3080,7 +3095,7 @@
       <c r="V21" s="14"/>
     </row>
     <row r="22" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
+      <c r="A22" s="78"/>
       <c r="B22" s="22" t="s">
         <v>14</v>
       </c>
@@ -3106,7 +3121,7 @@
       <c r="V22" s="14"/>
     </row>
     <row r="23" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65"/>
+      <c r="A23" s="78"/>
       <c r="B23" s="22" t="s">
         <v>15</v>
       </c>
@@ -3132,7 +3147,7 @@
       <c r="V23" s="14"/>
     </row>
     <row r="24" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
+      <c r="A24" s="78"/>
       <c r="B24" s="22" t="s">
         <v>16</v>
       </c>
@@ -3158,7 +3173,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="85"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3184,7 +3199,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="84" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3212,7 +3227,7 @@
       <c r="V26" s="21"/>
     </row>
     <row r="27" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="22" t="s">
         <v>12</v>
       </c>
@@ -3238,7 +3253,7 @@
       <c r="V27" s="14"/>
     </row>
     <row r="28" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="22" t="s">
         <v>13</v>
       </c>
@@ -3264,7 +3279,7 @@
       <c r="V28" s="14"/>
     </row>
     <row r="29" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="22" t="s">
         <v>14</v>
       </c>
@@ -3290,7 +3305,7 @@
       <c r="V29" s="14"/>
     </row>
     <row r="30" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="22" t="s">
         <v>15</v>
       </c>
@@ -3316,7 +3331,7 @@
       <c r="V30" s="14"/>
     </row>
     <row r="31" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="65"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="22" t="s">
         <v>16</v>
       </c>
@@ -3342,7 +3357,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
+      <c r="A32" s="85"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3368,7 +3383,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="84" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3396,7 +3411,7 @@
       <c r="V33" s="21"/>
     </row>
     <row r="34" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65"/>
+      <c r="A34" s="78"/>
       <c r="B34" s="22" t="s">
         <v>12</v>
       </c>
@@ -3422,7 +3437,7 @@
       <c r="V34" s="14"/>
     </row>
     <row r="35" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
+      <c r="A35" s="78"/>
       <c r="B35" s="22" t="s">
         <v>13</v>
       </c>
@@ -3448,7 +3463,7 @@
       <c r="V35" s="14"/>
     </row>
     <row r="36" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
+      <c r="A36" s="78"/>
       <c r="B36" s="22" t="s">
         <v>14</v>
       </c>
@@ -3474,7 +3489,7 @@
       <c r="V36" s="14"/>
     </row>
     <row r="37" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="65"/>
+      <c r="A37" s="78"/>
       <c r="B37" s="22" t="s">
         <v>15</v>
       </c>
@@ -3500,7 +3515,7 @@
       <c r="V37" s="14"/>
     </row>
     <row r="38" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="65"/>
+      <c r="A38" s="78"/>
       <c r="B38" s="22" t="s">
         <v>16</v>
       </c>
@@ -3526,7 +3541,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
+      <c r="A39" s="85"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3552,7 +3567,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="77" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3580,7 +3595,7 @@
       <c r="V40" s="21"/>
     </row>
     <row r="41" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="65"/>
+      <c r="A41" s="78"/>
       <c r="B41" s="22" t="s">
         <v>12</v>
       </c>
@@ -3606,7 +3621,7 @@
       <c r="V41" s="14"/>
     </row>
     <row r="42" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="22" t="s">
         <v>13</v>
       </c>
@@ -3632,7 +3647,7 @@
       <c r="V42" s="14"/>
     </row>
     <row r="43" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="65"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="22" t="s">
         <v>14</v>
       </c>
@@ -3658,7 +3673,7 @@
       <c r="V43" s="14"/>
     </row>
     <row r="44" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="65"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="22" t="s">
         <v>15</v>
       </c>
@@ -3684,7 +3699,7 @@
       <c r="V44" s="14"/>
     </row>
     <row r="45" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="22" t="s">
         <v>16</v>
       </c>
@@ -3710,7 +3725,7 @@
       <c r="V45" s="14"/>
     </row>
     <row r="46" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="23" t="s">
         <v>17</v>
       </c>
@@ -3736,7 +3751,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="64" t="s">
+      <c r="A47" s="84" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3764,7 +3779,7 @@
       <c r="V47" s="21"/>
     </row>
     <row r="48" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="22" t="s">
         <v>12</v>
       </c>
@@ -3790,7 +3805,7 @@
       <c r="V48" s="14"/>
     </row>
     <row r="49" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="65"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="22" t="s">
         <v>13</v>
       </c>
@@ -3816,7 +3831,7 @@
       <c r="V49" s="14"/>
     </row>
     <row r="50" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="65"/>
+      <c r="A50" s="78"/>
       <c r="B50" s="22" t="s">
         <v>14</v>
       </c>
@@ -3842,7 +3857,7 @@
       <c r="V50" s="14"/>
     </row>
     <row r="51" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
+      <c r="A51" s="78"/>
       <c r="B51" s="22" t="s">
         <v>15</v>
       </c>
@@ -3868,7 +3883,7 @@
       <c r="V51" s="14"/>
     </row>
     <row r="52" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
+      <c r="A52" s="78"/>
       <c r="B52" s="22" t="s">
         <v>16</v>
       </c>
@@ -3894,7 +3909,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="66"/>
+      <c r="A53" s="85"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3920,7 +3935,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="77" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -3948,7 +3963,7 @@
       <c r="V54" s="21"/>
     </row>
     <row r="55" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
+      <c r="A55" s="78"/>
       <c r="B55" s="22" t="s">
         <v>12</v>
       </c>
@@ -3974,7 +3989,7 @@
       <c r="V55" s="14"/>
     </row>
     <row r="56" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="65"/>
+      <c r="A56" s="78"/>
       <c r="B56" s="22" t="s">
         <v>13</v>
       </c>
@@ -4000,7 +4015,7 @@
       <c r="V56" s="14"/>
     </row>
     <row r="57" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
+      <c r="A57" s="78"/>
       <c r="B57" s="22" t="s">
         <v>14</v>
       </c>
@@ -4026,7 +4041,7 @@
       <c r="V57" s="14"/>
     </row>
     <row r="58" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
+      <c r="A58" s="78"/>
       <c r="B58" s="22" t="s">
         <v>15</v>
       </c>
@@ -4052,7 +4067,7 @@
       <c r="V58" s="14"/>
     </row>
     <row r="59" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="78"/>
       <c r="B59" s="22" t="s">
         <v>16</v>
       </c>
@@ -4078,7 +4093,7 @@
       <c r="V59" s="14"/>
     </row>
     <row r="60" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="78"/>
       <c r="B60" s="23" t="s">
         <v>17</v>
       </c>
@@ -4104,7 +4119,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="64" t="s">
+      <c r="A61" s="84" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4132,7 +4147,7 @@
       <c r="V61" s="21"/>
     </row>
     <row r="62" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
+      <c r="A62" s="78"/>
       <c r="B62" s="22" t="s">
         <v>12</v>
       </c>
@@ -4158,7 +4173,7 @@
       <c r="V62" s="14"/>
     </row>
     <row r="63" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="78"/>
       <c r="B63" s="22" t="s">
         <v>13</v>
       </c>
@@ -4184,7 +4199,7 @@
       <c r="V63" s="14"/>
     </row>
     <row r="64" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="78"/>
       <c r="B64" s="22" t="s">
         <v>14</v>
       </c>
@@ -4210,7 +4225,7 @@
       <c r="V64" s="14"/>
     </row>
     <row r="65" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="78"/>
       <c r="B65" s="22" t="s">
         <v>15</v>
       </c>
@@ -4236,7 +4251,7 @@
       <c r="V65" s="14"/>
     </row>
     <row r="66" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
+      <c r="A66" s="78"/>
       <c r="B66" s="22" t="s">
         <v>16</v>
       </c>
@@ -4262,7 +4277,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="66"/>
+      <c r="A67" s="85"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4288,7 +4303,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="64" t="s">
+      <c r="A68" s="84" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4316,7 +4331,7 @@
       <c r="V68" s="21"/>
     </row>
     <row r="69" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="78"/>
       <c r="B69" s="22" t="s">
         <v>12</v>
       </c>
@@ -4342,7 +4357,7 @@
       <c r="V69" s="14"/>
     </row>
     <row r="70" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="78"/>
       <c r="B70" s="22" t="s">
         <v>13</v>
       </c>
@@ -4368,7 +4383,7 @@
       <c r="V70" s="14"/>
     </row>
     <row r="71" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="22" t="s">
         <v>14</v>
       </c>
@@ -4394,7 +4409,7 @@
       <c r="V71" s="14"/>
     </row>
     <row r="72" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="22" t="s">
         <v>15</v>
       </c>
@@ -4420,7 +4435,7 @@
       <c r="V72" s="14"/>
     </row>
     <row r="73" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
+      <c r="A73" s="78"/>
       <c r="B73" s="22" t="s">
         <v>16</v>
       </c>
@@ -4446,7 +4461,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="66"/>
+      <c r="A74" s="85"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4472,7 +4487,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="67" t="s">
+      <c r="A75" s="77" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4500,7 +4515,7 @@
       <c r="V75" s="21"/>
     </row>
     <row r="76" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="78"/>
       <c r="B76" s="22" t="s">
         <v>12</v>
       </c>
@@ -4526,7 +4541,7 @@
       <c r="V76" s="14"/>
     </row>
     <row r="77" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="78"/>
       <c r="B77" s="22" t="s">
         <v>13</v>
       </c>
@@ -4552,7 +4567,7 @@
       <c r="V77" s="14"/>
     </row>
     <row r="78" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="78"/>
       <c r="B78" s="22" t="s">
         <v>14</v>
       </c>
@@ -4578,7 +4593,7 @@
       <c r="V78" s="14"/>
     </row>
     <row r="79" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
+      <c r="A79" s="78"/>
       <c r="B79" s="22" t="s">
         <v>15</v>
       </c>
@@ -4604,7 +4619,7 @@
       <c r="V79" s="14"/>
     </row>
     <row r="80" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="65"/>
+      <c r="A80" s="78"/>
       <c r="B80" s="22" t="s">
         <v>16</v>
       </c>
@@ -4630,7 +4645,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="68"/>
+      <c r="A81" s="87"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4657,23 +4672,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4688,7 +4703,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4699,128 +4714,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="82" t="s">
+      <c r="C1" s="93"/>
+      <c r="D1" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="78" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="77" t="s">
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="78" t="s">
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="77" t="s">
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="78" t="s">
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="90"/>
+      <c r="AJ1" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="78"/>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="78"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="77" t="s">
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="78" t="s">
+      <c r="AQ1" s="90"/>
+      <c r="AR1" s="90"/>
+      <c r="AS1" s="90"/>
+      <c r="AT1" s="90"/>
+      <c r="AU1" s="90"/>
+      <c r="AV1" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="78"/>
-      <c r="AX1" s="78"/>
-      <c r="AY1" s="78"/>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="78"/>
-      <c r="BB1" s="77" t="s">
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="91"/>
+      <c r="AY1" s="91"/>
+      <c r="AZ1" s="91"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="77"/>
-      <c r="BF1" s="77"/>
-      <c r="BG1" s="77"/>
-      <c r="BH1" s="78" t="s">
+      <c r="BC1" s="90"/>
+      <c r="BD1" s="90"/>
+      <c r="BE1" s="90"/>
+      <c r="BF1" s="90"/>
+      <c r="BG1" s="90"/>
+      <c r="BH1" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="BI1" s="78"/>
-      <c r="BJ1" s="78"/>
-      <c r="BK1" s="78"/>
-      <c r="BL1" s="78"/>
-      <c r="BM1" s="78"/>
-      <c r="BN1" s="77" t="s">
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="91"/>
+      <c r="BK1" s="91"/>
+      <c r="BL1" s="91"/>
+      <c r="BM1" s="91"/>
+      <c r="BN1" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" s="77"/>
-      <c r="BP1" s="77"/>
-      <c r="BQ1" s="77"/>
-      <c r="BR1" s="77"/>
-      <c r="BS1" s="83"/>
+      <c r="BO1" s="90"/>
+      <c r="BP1" s="90"/>
+      <c r="BQ1" s="90"/>
+      <c r="BR1" s="90"/>
+      <c r="BS1" s="96"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
+      <c r="A2" s="89"/>
       <c r="B2" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81" t="s">
+      <c r="D2" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="81"/>
+      <c r="K2" s="94"/>
       <c r="L2" s="26" t="s">
         <v>29</v>
       </c>
@@ -5012,10 +5027,10 @@
       <c r="C3" s="37">
         <v>9</v>
       </c>
-      <c r="D3" s="91">
-        <v>0</v>
-      </c>
-      <c r="E3" s="89">
+      <c r="D3" s="69">
+        <v>0</v>
+      </c>
+      <c r="E3" s="67">
         <v>0</v>
       </c>
       <c r="F3" s="28">
@@ -5024,16 +5039,16 @@
       <c r="G3" s="28">
         <v>16</v>
       </c>
-      <c r="H3" s="89">
-        <v>0</v>
-      </c>
-      <c r="I3" s="89">
-        <v>0</v>
-      </c>
-      <c r="J3" s="89">
-        <v>0</v>
-      </c>
-      <c r="K3" s="90">
+      <c r="H3" s="67">
+        <v>0</v>
+      </c>
+      <c r="I3" s="67">
+        <v>0</v>
+      </c>
+      <c r="J3" s="67">
+        <v>0</v>
+      </c>
+      <c r="K3" s="68">
         <v>0</v>
       </c>
       <c r="L3" s="40">
@@ -5359,76 +5374,76 @@
       <c r="AU4" s="30">
         <v>60</v>
       </c>
-      <c r="AV4" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY4" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA4" s="86">
+      <c r="AV4" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="64">
         <v>60</v>
       </c>
-      <c r="BB4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG4" s="85">
+      <c r="BB4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="63">
         <v>60</v>
       </c>
-      <c r="BH4" s="84">
-        <v>0</v>
-      </c>
-      <c r="BI4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="86">
+      <c r="BH4" s="62">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="64">
         <v>40</v>
       </c>
-      <c r="BN4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS4" s="87">
+      <c r="BN4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS4" s="65">
         <v>45</v>
       </c>
     </row>
@@ -5442,22 +5457,22 @@
       <c r="C5" s="38">
         <v>9</v>
       </c>
-      <c r="D5" s="84">
-        <v>0</v>
-      </c>
-      <c r="E5" s="85">
-        <v>0</v>
-      </c>
-      <c r="F5" s="85">
-        <v>0</v>
-      </c>
-      <c r="G5" s="85">
-        <v>0</v>
-      </c>
-      <c r="H5" s="85">
-        <v>0</v>
-      </c>
-      <c r="I5" s="85">
+      <c r="D5" s="62">
+        <v>0</v>
+      </c>
+      <c r="E5" s="63">
+        <v>0</v>
+      </c>
+      <c r="F5" s="63">
+        <v>0</v>
+      </c>
+      <c r="G5" s="63">
+        <v>0</v>
+      </c>
+      <c r="H5" s="63">
+        <v>0</v>
+      </c>
+      <c r="I5" s="63">
         <v>0</v>
       </c>
       <c r="J5" s="30">
@@ -5574,76 +5589,76 @@
       <c r="AU5" s="30">
         <v>50</v>
       </c>
-      <c r="AV5" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="86">
+      <c r="AV5" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="64">
         <v>60</v>
       </c>
-      <c r="BB5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="85">
+      <c r="BB5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="63">
         <v>60</v>
       </c>
-      <c r="BH5" s="84">
-        <v>0</v>
-      </c>
-      <c r="BI5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM5" s="86">
+      <c r="BH5" s="62">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="64">
         <v>60</v>
       </c>
-      <c r="BN5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR5" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS5" s="87">
+      <c r="BN5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS5" s="65">
         <v>45</v>
       </c>
     </row>
@@ -5657,10 +5672,10 @@
       <c r="C6" s="38">
         <v>9</v>
       </c>
-      <c r="D6" s="84">
-        <v>0</v>
-      </c>
-      <c r="E6" s="85">
+      <c r="D6" s="62">
+        <v>0</v>
+      </c>
+      <c r="E6" s="63">
         <v>0</v>
       </c>
       <c r="F6" s="30">
@@ -5669,10 +5684,10 @@
       <c r="G6" s="30">
         <v>16</v>
       </c>
-      <c r="H6" s="85">
-        <v>0</v>
-      </c>
-      <c r="I6" s="85">
+      <c r="H6" s="63">
+        <v>0</v>
+      </c>
+      <c r="I6" s="63">
         <v>0</v>
       </c>
       <c r="J6" s="30">
@@ -5771,94 +5786,94 @@
       <c r="AO6" s="43">
         <v>90</v>
       </c>
-      <c r="AP6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="85">
+      <c r="AP6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="63">
         <v>25</v>
       </c>
-      <c r="AV6" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY6" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="86">
+      <c r="AV6" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="64">
         <v>30</v>
       </c>
-      <c r="BB6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG6" s="85">
+      <c r="BB6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="63">
         <v>35</v>
       </c>
-      <c r="BH6" s="84">
+      <c r="BH6" s="62">
         <v>8</v>
       </c>
-      <c r="BI6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM6" s="86">
+      <c r="BI6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="64">
         <v>40</v>
       </c>
-      <c r="BN6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR6" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS6" s="87">
+      <c r="BN6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR6" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS6" s="65">
         <v>45</v>
       </c>
     </row>
@@ -5872,10 +5887,10 @@
       <c r="C7" s="38">
         <v>8</v>
       </c>
-      <c r="D7" s="84">
-        <v>0</v>
-      </c>
-      <c r="E7" s="85">
+      <c r="D7" s="62">
+        <v>0</v>
+      </c>
+      <c r="E7" s="63">
         <v>0</v>
       </c>
       <c r="F7" s="30">
@@ -6040,40 +6055,40 @@
       <c r="BG7" s="30">
         <v>70</v>
       </c>
-      <c r="BH7" s="84">
-        <v>0</v>
-      </c>
-      <c r="BI7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="86">
+      <c r="BH7" s="62">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="64">
         <v>40</v>
       </c>
-      <c r="BN7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR7" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS7" s="87">
+      <c r="BN7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR7" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS7" s="65">
         <v>45</v>
       </c>
     </row>
@@ -6219,76 +6234,76 @@
       <c r="AU8" s="30">
         <v>70</v>
       </c>
-      <c r="AV8" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="86">
+      <c r="AV8" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="64">
         <v>30</v>
       </c>
-      <c r="BB8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="85">
+      <c r="BB8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="63">
         <v>35</v>
       </c>
-      <c r="BH8" s="84">
-        <v>0</v>
-      </c>
-      <c r="BI8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="86">
+      <c r="BH8" s="62">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="64">
         <v>40</v>
       </c>
-      <c r="BN8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR8" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS8" s="87">
+      <c r="BN8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR8" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS8" s="65">
         <v>45</v>
       </c>
     </row>
@@ -6302,10 +6317,10 @@
       <c r="C9" s="38">
         <v>13</v>
       </c>
-      <c r="D9" s="84">
-        <v>0</v>
-      </c>
-      <c r="E9" s="85">
+      <c r="D9" s="62">
+        <v>0</v>
+      </c>
+      <c r="E9" s="63">
         <v>0</v>
       </c>
       <c r="F9" s="30">
@@ -6314,10 +6329,10 @@
       <c r="G9" s="30">
         <v>16</v>
       </c>
-      <c r="H9" s="85">
-        <v>0</v>
-      </c>
-      <c r="I9" s="85">
+      <c r="H9" s="63">
+        <v>0</v>
+      </c>
+      <c r="I9" s="63">
         <v>0</v>
       </c>
       <c r="J9" s="30">
@@ -6452,58 +6467,58 @@
       <c r="BA9" s="43">
         <v>120</v>
       </c>
-      <c r="BB9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="85">
+      <c r="BB9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="63">
         <v>35</v>
       </c>
-      <c r="BH9" s="84">
+      <c r="BH9" s="62">
         <v>8</v>
       </c>
-      <c r="BI9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM9" s="86">
+      <c r="BI9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="64">
         <v>40</v>
       </c>
-      <c r="BN9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR9" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS9" s="87">
+      <c r="BN9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR9" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS9" s="65">
         <v>45</v>
       </c>
     </row>
@@ -6535,10 +6550,10 @@
       <c r="I10" s="30">
         <v>28</v>
       </c>
-      <c r="J10" s="85">
-        <v>0</v>
-      </c>
-      <c r="K10" s="88">
+      <c r="J10" s="63">
+        <v>0</v>
+      </c>
+      <c r="K10" s="66">
         <v>0</v>
       </c>
       <c r="L10" s="42">
@@ -6631,94 +6646,94 @@
       <c r="AO10" s="43">
         <v>90</v>
       </c>
-      <c r="AP10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="85">
+      <c r="AP10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="63">
         <v>25</v>
       </c>
-      <c r="AV10" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="86">
+      <c r="AV10" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="64">
         <v>30</v>
       </c>
-      <c r="BB10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BC10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG10" s="85">
+      <c r="BB10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="63">
         <v>35</v>
       </c>
-      <c r="BH10" s="84">
-        <v>0</v>
-      </c>
-      <c r="BI10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM10" s="86">
+      <c r="BH10" s="62">
+        <v>0</v>
+      </c>
+      <c r="BI10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="64">
         <v>40</v>
       </c>
-      <c r="BN10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR10" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS10" s="87">
+      <c r="BN10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR10" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS10" s="65">
         <v>45</v>
       </c>
     </row>
@@ -6732,10 +6747,10 @@
       <c r="C11" s="38">
         <v>9</v>
       </c>
-      <c r="D11" s="84">
-        <v>0</v>
-      </c>
-      <c r="E11" s="85">
+      <c r="D11" s="62">
+        <v>0</v>
+      </c>
+      <c r="E11" s="63">
         <v>0</v>
       </c>
       <c r="F11" s="30">
@@ -6744,10 +6759,10 @@
       <c r="G11" s="30">
         <v>15</v>
       </c>
-      <c r="H11" s="85">
-        <v>0</v>
-      </c>
-      <c r="I11" s="85">
+      <c r="H11" s="63">
+        <v>0</v>
+      </c>
+      <c r="I11" s="63">
         <v>0</v>
       </c>
       <c r="J11" s="30">
@@ -7061,130 +7076,130 @@
       <c r="AO12" s="43">
         <v>80</v>
       </c>
-      <c r="AP12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="85">
+      <c r="AP12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="63">
         <v>25</v>
       </c>
-      <c r="AV12" s="84">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AY12" s="85">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BA12" s="86">
+      <c r="AV12" s="62">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BA12" s="64">
         <v>30</v>
       </c>
-      <c r="BB12" s="85">
+      <c r="BB12" s="63">
         <v>7</v>
       </c>
-      <c r="BC12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BF12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BG12" s="85">
+      <c r="BC12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BD12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BE12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BF12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BG12" s="63">
         <v>35</v>
       </c>
-      <c r="BH12" s="84">
+      <c r="BH12" s="62">
         <v>8</v>
       </c>
-      <c r="BI12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BK12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BM12" s="86">
+      <c r="BI12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BJ12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BK12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BM12" s="64">
         <v>40</v>
       </c>
-      <c r="BN12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BR12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BS12" s="87">
+      <c r="BN12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BP12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BR12" s="63">
+        <v>0</v>
+      </c>
+      <c r="BS12" s="65">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46">
+      <c r="A13" s="70">
         <v>11</v>
       </c>
-      <c r="B13" s="47">
-        <v>10</v>
-      </c>
-      <c r="C13" s="48">
-        <v>10</v>
-      </c>
-      <c r="D13" s="49">
-        <v>5</v>
-      </c>
-      <c r="E13" s="50">
-        <v>25</v>
-      </c>
-      <c r="F13" s="50">
-        <v>4</v>
-      </c>
-      <c r="G13" s="50">
-        <v>14</v>
-      </c>
-      <c r="H13" s="50">
-        <v>5</v>
-      </c>
-      <c r="I13" s="50">
-        <v>25</v>
-      </c>
-      <c r="J13" s="50">
-        <v>4</v>
-      </c>
-      <c r="K13" s="48">
-        <v>14</v>
+      <c r="B13" s="71">
+        <v>15</v>
+      </c>
+      <c r="C13" s="72">
+        <v>9</v>
+      </c>
+      <c r="D13" s="73">
+        <v>2</v>
+      </c>
+      <c r="E13" s="74">
+        <v>28</v>
+      </c>
+      <c r="F13" s="74">
+        <v>2</v>
+      </c>
+      <c r="G13" s="74">
+        <v>16</v>
+      </c>
+      <c r="H13" s="74">
+        <v>2</v>
+      </c>
+      <c r="I13" s="74">
+        <v>28</v>
+      </c>
+      <c r="J13" s="74">
+        <v>2</v>
+      </c>
+      <c r="K13" s="72">
+        <v>16</v>
       </c>
       <c r="L13" s="49">
         <v>0</v>
@@ -7226,16 +7241,16 @@
         <v>2</v>
       </c>
       <c r="Y13" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z13" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA13" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB13" s="50">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AC13" s="51">
         <v>10</v>
@@ -7368,53 +7383,53 @@
       </c>
     </row>
     <row r="14" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="70">
         <v>12</v>
       </c>
-      <c r="B14" s="47">
-        <v>10</v>
-      </c>
-      <c r="C14" s="48">
-        <v>10</v>
-      </c>
-      <c r="D14" s="49">
-        <v>5</v>
-      </c>
-      <c r="E14" s="50">
+      <c r="B14" s="71">
+        <v>3</v>
+      </c>
+      <c r="C14" s="72">
+        <v>11</v>
+      </c>
+      <c r="D14" s="73">
+        <v>5</v>
+      </c>
+      <c r="E14" s="74">
         <v>25</v>
       </c>
-      <c r="F14" s="50">
-        <v>4</v>
-      </c>
-      <c r="G14" s="50">
-        <v>14</v>
+      <c r="F14" s="74">
+        <v>2</v>
+      </c>
+      <c r="G14" s="74">
+        <v>16</v>
       </c>
       <c r="H14" s="50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I14" s="50">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J14" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K14" s="48">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L14" s="49">
         <v>0</v>
       </c>
       <c r="M14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O14" s="50">
         <v>0</v>
       </c>
       <c r="P14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="51">
         <v>0</v>
@@ -7423,16 +7438,16 @@
         <v>1</v>
       </c>
       <c r="S14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U14" s="50">
         <v>0</v>
       </c>
       <c r="V14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W14" s="50">
         <v>5</v>
@@ -7441,16 +7456,16 @@
         <v>2</v>
       </c>
       <c r="Y14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA14" s="50">
         <v>0</v>
       </c>
       <c r="AB14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="51">
         <v>10</v>
@@ -7459,16 +7474,16 @@
         <v>3</v>
       </c>
       <c r="AE14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG14" s="50">
         <v>0</v>
       </c>
       <c r="AH14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="50">
         <v>15</v>
@@ -7477,16 +7492,16 @@
         <v>4</v>
       </c>
       <c r="AK14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM14" s="50">
         <v>0</v>
       </c>
       <c r="AN14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="51">
         <v>20</v>
@@ -7495,16 +7510,16 @@
         <v>5</v>
       </c>
       <c r="AQ14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS14" s="50">
         <v>0</v>
       </c>
       <c r="AT14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU14" s="50">
         <v>25</v>
@@ -7513,16 +7528,16 @@
         <v>6</v>
       </c>
       <c r="AW14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY14" s="50">
         <v>0</v>
       </c>
       <c r="AZ14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA14" s="51">
         <v>30</v>
@@ -7531,16 +7546,16 @@
         <v>7</v>
       </c>
       <c r="BC14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE14" s="50">
         <v>0</v>
       </c>
       <c r="BF14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG14" s="50">
         <v>35</v>
@@ -7549,16 +7564,16 @@
         <v>8</v>
       </c>
       <c r="BI14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BJ14" s="50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BK14" s="50">
         <v>0</v>
       </c>
       <c r="BL14" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BM14" s="51">
         <v>40</v>
@@ -7583,38 +7598,38 @@
       </c>
     </row>
     <row r="15" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46">
+      <c r="A15" s="70">
         <v>13</v>
       </c>
-      <c r="B15" s="47">
-        <v>10</v>
-      </c>
-      <c r="C15" s="48">
-        <v>10</v>
+      <c r="B15" s="71">
+        <v>15</v>
+      </c>
+      <c r="C15" s="72">
+        <v>3</v>
       </c>
       <c r="D15" s="49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E15" s="50">
-        <v>25</v>
-      </c>
-      <c r="F15" s="50">
-        <v>4</v>
-      </c>
-      <c r="G15" s="50">
+        <v>0</v>
+      </c>
+      <c r="F15" s="74">
+        <v>15</v>
+      </c>
+      <c r="G15" s="74">
+        <v>16</v>
+      </c>
+      <c r="H15" s="74">
+        <v>15</v>
+      </c>
+      <c r="I15" s="74">
+        <v>16</v>
+      </c>
+      <c r="J15" s="74">
         <v>14</v>
       </c>
-      <c r="H15" s="50">
-        <v>5</v>
-      </c>
-      <c r="I15" s="50">
-        <v>25</v>
-      </c>
-      <c r="J15" s="50">
-        <v>4</v>
-      </c>
-      <c r="K15" s="48">
-        <v>14</v>
+      <c r="K15" s="72">
+        <v>16</v>
       </c>
       <c r="L15" s="49">
         <v>0</v>
@@ -7623,10 +7638,10 @@
         <v>0</v>
       </c>
       <c r="N15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P15" s="50">
         <v>3</v>
@@ -7641,10 +7656,10 @@
         <v>0</v>
       </c>
       <c r="T15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V15" s="50">
         <v>3</v>
@@ -7659,10 +7674,10 @@
         <v>0</v>
       </c>
       <c r="Z15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB15" s="50">
         <v>3</v>
@@ -7677,10 +7692,10 @@
         <v>0</v>
       </c>
       <c r="AF15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="50">
         <v>3</v>
@@ -7695,10 +7710,10 @@
         <v>0</v>
       </c>
       <c r="AL15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN15" s="50">
         <v>3</v>
@@ -7713,10 +7728,10 @@
         <v>0</v>
       </c>
       <c r="AR15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT15" s="50">
         <v>3</v>
@@ -7731,10 +7746,10 @@
         <v>0</v>
       </c>
       <c r="AX15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AY15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ15" s="50">
         <v>3</v>
@@ -7749,10 +7764,10 @@
         <v>0</v>
       </c>
       <c r="BD15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF15" s="50">
         <v>3</v>
@@ -7767,10 +7782,10 @@
         <v>0</v>
       </c>
       <c r="BJ15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK15" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL15" s="50">
         <v>3</v>
@@ -7798,38 +7813,38 @@
       </c>
     </row>
     <row r="16" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46">
+      <c r="A16" s="70">
         <v>14</v>
       </c>
-      <c r="B16" s="47">
-        <v>10</v>
-      </c>
-      <c r="C16" s="48">
-        <v>10</v>
-      </c>
-      <c r="D16" s="49">
-        <v>5</v>
-      </c>
-      <c r="E16" s="50">
-        <v>25</v>
-      </c>
-      <c r="F16" s="50">
-        <v>4</v>
-      </c>
-      <c r="G16" s="50">
-        <v>14</v>
-      </c>
-      <c r="H16" s="50">
-        <v>5</v>
-      </c>
-      <c r="I16" s="50">
-        <v>25</v>
-      </c>
-      <c r="J16" s="50">
-        <v>4</v>
-      </c>
-      <c r="K16" s="48">
-        <v>14</v>
+      <c r="B16" s="71">
+        <v>15</v>
+      </c>
+      <c r="C16" s="72">
+        <v>6</v>
+      </c>
+      <c r="D16" s="73">
+        <v>2</v>
+      </c>
+      <c r="E16" s="74">
+        <v>28</v>
+      </c>
+      <c r="F16" s="74">
+        <v>11</v>
+      </c>
+      <c r="G16" s="74">
+        <v>12</v>
+      </c>
+      <c r="H16" s="74">
+        <v>2</v>
+      </c>
+      <c r="I16" s="74">
+        <v>28</v>
+      </c>
+      <c r="J16" s="74">
+        <v>11</v>
+      </c>
+      <c r="K16" s="72">
+        <v>12</v>
       </c>
       <c r="L16" s="49">
         <v>0</v>
@@ -7871,16 +7886,16 @@
         <v>2</v>
       </c>
       <c r="Y16" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z16" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA16" s="50">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB16" s="50">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AC16" s="51">
         <v>10</v>
@@ -8013,50 +8028,50 @@
       </c>
     </row>
     <row r="17" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46">
+      <c r="A17" s="70">
         <v>15</v>
       </c>
-      <c r="B17" s="47">
-        <v>10</v>
-      </c>
-      <c r="C17" s="48">
-        <v>10</v>
-      </c>
-      <c r="D17" s="49">
-        <v>5</v>
-      </c>
-      <c r="E17" s="50">
+      <c r="B17" s="71">
+        <v>28</v>
+      </c>
+      <c r="C17" s="72">
+        <v>10</v>
+      </c>
+      <c r="D17" s="73">
+        <v>5</v>
+      </c>
+      <c r="E17" s="74">
         <v>25</v>
       </c>
       <c r="F17" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G17" s="50">
-        <v>14</v>
-      </c>
-      <c r="H17" s="50">
-        <v>5</v>
-      </c>
-      <c r="I17" s="50">
-        <v>25</v>
-      </c>
-      <c r="J17" s="50">
-        <v>4</v>
-      </c>
-      <c r="K17" s="48">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="H17" s="74">
+        <v>8</v>
+      </c>
+      <c r="I17" s="74">
+        <v>15</v>
+      </c>
+      <c r="J17" s="74">
+        <v>9</v>
+      </c>
+      <c r="K17" s="72">
+        <v>12</v>
       </c>
       <c r="L17" s="49">
         <v>0</v>
       </c>
       <c r="M17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N17" s="50">
         <v>0</v>
       </c>
       <c r="O17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P17" s="50">
         <v>3</v>
@@ -8068,13 +8083,13 @@
         <v>1</v>
       </c>
       <c r="S17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T17" s="50">
         <v>0</v>
       </c>
       <c r="U17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V17" s="50">
         <v>3</v>
@@ -8086,13 +8101,13 @@
         <v>2</v>
       </c>
       <c r="Y17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z17" s="50">
         <v>0</v>
       </c>
       <c r="AA17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB17" s="50">
         <v>3</v>
@@ -8104,13 +8119,13 @@
         <v>3</v>
       </c>
       <c r="AE17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF17" s="50">
         <v>0</v>
       </c>
       <c r="AG17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH17" s="50">
         <v>3</v>
@@ -8122,13 +8137,13 @@
         <v>4</v>
       </c>
       <c r="AK17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL17" s="50">
         <v>0</v>
       </c>
       <c r="AM17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN17" s="50">
         <v>3</v>
@@ -8140,13 +8155,13 @@
         <v>5</v>
       </c>
       <c r="AQ17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR17" s="50">
         <v>0</v>
       </c>
       <c r="AS17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT17" s="50">
         <v>3</v>
@@ -8158,13 +8173,13 @@
         <v>6</v>
       </c>
       <c r="AW17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX17" s="50">
         <v>0</v>
       </c>
       <c r="AY17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ17" s="50">
         <v>3</v>
@@ -8176,13 +8191,13 @@
         <v>7</v>
       </c>
       <c r="BC17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD17" s="50">
         <v>0</v>
       </c>
       <c r="BE17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF17" s="50">
         <v>3</v>
@@ -8194,13 +8209,13 @@
         <v>8</v>
       </c>
       <c r="BI17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ17" s="50">
         <v>0</v>
       </c>
       <c r="BK17" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL17" s="50">
         <v>3</v>
@@ -8228,53 +8243,53 @@
       </c>
     </row>
     <row r="18" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+      <c r="A18" s="70">
         <v>16</v>
       </c>
-      <c r="B18" s="47">
-        <v>10</v>
-      </c>
-      <c r="C18" s="48">
-        <v>10</v>
-      </c>
-      <c r="D18" s="49">
-        <v>5</v>
-      </c>
-      <c r="E18" s="50">
-        <v>25</v>
+      <c r="B18" s="71">
+        <v>20</v>
+      </c>
+      <c r="C18" s="72">
+        <v>10</v>
+      </c>
+      <c r="D18" s="73">
+        <v>2</v>
+      </c>
+      <c r="E18" s="74">
+        <v>3</v>
       </c>
       <c r="F18" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G18" s="50">
-        <v>14</v>
-      </c>
-      <c r="H18" s="50">
-        <v>5</v>
-      </c>
-      <c r="I18" s="50">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="H18" s="74">
+        <v>1</v>
+      </c>
+      <c r="I18" s="74">
+        <v>8</v>
       </c>
       <c r="J18" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K18" s="48">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L18" s="49">
         <v>0</v>
       </c>
       <c r="M18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N18" s="50">
         <v>0</v>
       </c>
       <c r="O18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="51">
         <v>0</v>
@@ -8283,16 +8298,16 @@
         <v>1</v>
       </c>
       <c r="S18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T18" s="50">
         <v>0</v>
       </c>
       <c r="U18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W18" s="50">
         <v>5</v>
@@ -8301,16 +8316,16 @@
         <v>2</v>
       </c>
       <c r="Y18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z18" s="50">
         <v>0</v>
       </c>
       <c r="AA18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="51">
         <v>10</v>
@@ -8319,16 +8334,16 @@
         <v>3</v>
       </c>
       <c r="AE18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF18" s="50">
         <v>0</v>
       </c>
       <c r="AG18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI18" s="50">
         <v>15</v>
@@ -8337,16 +8352,16 @@
         <v>4</v>
       </c>
       <c r="AK18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL18" s="50">
         <v>0</v>
       </c>
       <c r="AM18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO18" s="51">
         <v>20</v>
@@ -8355,16 +8370,16 @@
         <v>5</v>
       </c>
       <c r="AQ18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR18" s="50">
         <v>0</v>
       </c>
       <c r="AS18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU18" s="50">
         <v>25</v>
@@ -8373,16 +8388,16 @@
         <v>6</v>
       </c>
       <c r="AW18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX18" s="50">
         <v>0</v>
       </c>
       <c r="AY18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA18" s="51">
         <v>30</v>
@@ -8391,16 +8406,16 @@
         <v>7</v>
       </c>
       <c r="BC18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD18" s="50">
         <v>0</v>
       </c>
       <c r="BE18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG18" s="50">
         <v>35</v>
@@ -8409,16 +8424,16 @@
         <v>8</v>
       </c>
       <c r="BI18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ18" s="50">
         <v>0</v>
       </c>
       <c r="BK18" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL18" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BM18" s="51">
         <v>40</v>
@@ -8443,44 +8458,44 @@
       </c>
     </row>
     <row r="19" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46">
+      <c r="A19" s="70">
         <v>17</v>
       </c>
-      <c r="B19" s="47">
-        <v>10</v>
-      </c>
-      <c r="C19" s="48">
-        <v>10</v>
-      </c>
-      <c r="D19" s="49">
-        <v>5</v>
-      </c>
-      <c r="E19" s="50">
-        <v>25</v>
+      <c r="B19" s="71">
+        <v>17</v>
+      </c>
+      <c r="C19" s="72">
+        <v>15</v>
+      </c>
+      <c r="D19" s="73">
+        <v>15</v>
+      </c>
+      <c r="E19" s="74">
+        <v>28</v>
       </c>
       <c r="F19" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G19" s="50">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H19" s="50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I19" s="50">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J19" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K19" s="48">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L19" s="49">
         <v>0</v>
       </c>
       <c r="M19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N19" s="50">
         <v>0</v>
@@ -8489,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="51">
         <v>0</v>
@@ -8498,7 +8513,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T19" s="50">
         <v>0</v>
@@ -8507,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W19" s="50">
         <v>5</v>
@@ -8516,7 +8531,7 @@
         <v>2</v>
       </c>
       <c r="Y19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z19" s="50">
         <v>0</v>
@@ -8525,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="51">
         <v>10</v>
@@ -8534,7 +8549,7 @@
         <v>3</v>
       </c>
       <c r="AE19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF19" s="50">
         <v>0</v>
@@ -8543,7 +8558,7 @@
         <v>0</v>
       </c>
       <c r="AH19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI19" s="50">
         <v>15</v>
@@ -8552,7 +8567,7 @@
         <v>4</v>
       </c>
       <c r="AK19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL19" s="50">
         <v>0</v>
@@ -8561,7 +8576,7 @@
         <v>0</v>
       </c>
       <c r="AN19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO19" s="51">
         <v>20</v>
@@ -8570,7 +8585,7 @@
         <v>5</v>
       </c>
       <c r="AQ19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR19" s="50">
         <v>0</v>
@@ -8579,7 +8594,7 @@
         <v>0</v>
       </c>
       <c r="AT19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU19" s="50">
         <v>25</v>
@@ -8588,7 +8603,7 @@
         <v>6</v>
       </c>
       <c r="AW19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX19" s="50">
         <v>0</v>
@@ -8597,7 +8612,7 @@
         <v>0</v>
       </c>
       <c r="AZ19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA19" s="51">
         <v>30</v>
@@ -8606,7 +8621,7 @@
         <v>7</v>
       </c>
       <c r="BC19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD19" s="50">
         <v>0</v>
@@ -8615,7 +8630,7 @@
         <v>0</v>
       </c>
       <c r="BF19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG19" s="50">
         <v>35</v>
@@ -8624,7 +8639,7 @@
         <v>8</v>
       </c>
       <c r="BI19" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ19" s="50">
         <v>0</v>
@@ -8633,7 +8648,7 @@
         <v>0</v>
       </c>
       <c r="BL19" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BM19" s="51">
         <v>40</v>
@@ -8658,44 +8673,44 @@
       </c>
     </row>
     <row r="20" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46">
+      <c r="A20" s="70">
         <v>18</v>
       </c>
-      <c r="B20" s="47">
-        <v>10</v>
-      </c>
-      <c r="C20" s="48">
-        <v>10</v>
-      </c>
-      <c r="D20" s="49">
-        <v>5</v>
-      </c>
-      <c r="E20" s="50">
-        <v>25</v>
+      <c r="B20" s="71">
+        <v>27</v>
+      </c>
+      <c r="C20" s="72">
+        <v>7</v>
+      </c>
+      <c r="D20" s="73">
+        <v>1</v>
+      </c>
+      <c r="E20" s="74">
+        <v>7</v>
       </c>
       <c r="F20" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G20" s="50">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H20" s="50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I20" s="50">
-        <v>25</v>
-      </c>
-      <c r="J20" s="50">
-        <v>4</v>
-      </c>
-      <c r="K20" s="48">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="J20" s="74">
+        <v>2</v>
+      </c>
+      <c r="K20" s="72">
+        <v>16</v>
       </c>
       <c r="L20" s="49">
         <v>0</v>
       </c>
       <c r="M20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N20" s="50">
         <v>0</v>
@@ -8713,7 +8728,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T20" s="50">
         <v>0</v>
@@ -8731,7 +8746,7 @@
         <v>2</v>
       </c>
       <c r="Y20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z20" s="50">
         <v>0</v>
@@ -8749,7 +8764,7 @@
         <v>3</v>
       </c>
       <c r="AE20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF20" s="50">
         <v>0</v>
@@ -8767,7 +8782,7 @@
         <v>4</v>
       </c>
       <c r="AK20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL20" s="50">
         <v>0</v>
@@ -8785,7 +8800,7 @@
         <v>5</v>
       </c>
       <c r="AQ20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR20" s="50">
         <v>0</v>
@@ -8803,7 +8818,7 @@
         <v>6</v>
       </c>
       <c r="AW20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX20" s="50">
         <v>0</v>
@@ -8821,7 +8836,7 @@
         <v>7</v>
       </c>
       <c r="BC20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD20" s="50">
         <v>0</v>
@@ -8839,7 +8854,7 @@
         <v>8</v>
       </c>
       <c r="BI20" s="50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ20" s="50">
         <v>0</v>
@@ -8873,38 +8888,38 @@
       </c>
     </row>
     <row r="21" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46">
+      <c r="A21" s="70">
         <v>19</v>
       </c>
-      <c r="B21" s="47">
-        <v>10</v>
-      </c>
-      <c r="C21" s="48">
-        <v>10</v>
+      <c r="B21" s="71">
+        <v>25</v>
+      </c>
+      <c r="C21" s="72">
+        <v>9</v>
       </c>
       <c r="D21" s="49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21" s="50">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F21" s="50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G21" s="50">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H21" s="50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I21" s="50">
-        <v>25</v>
-      </c>
-      <c r="J21" s="50">
-        <v>4</v>
-      </c>
-      <c r="K21" s="48">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="J21" s="74">
+        <v>2</v>
+      </c>
+      <c r="K21" s="72">
+        <v>16</v>
       </c>
       <c r="L21" s="49">
         <v>0</v>

</xml_diff>

<commit_message>
tuning level 1 -> 3
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1085,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1315,10 +1315,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1330,34 +1348,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1372,7 +1375,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2575,7 +2578,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="84" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2603,7 +2606,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2629,10 +2632,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2657,8 +2660,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2681,8 +2684,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
-      <c r="B6" s="79" t="s">
+      <c r="A6" s="87"/>
+      <c r="B6" s="85" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2707,8 +2710,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
-      <c r="B7" s="79"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2731,8 +2734,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
-      <c r="B8" s="79" t="s">
+      <c r="A8" s="87"/>
+      <c r="B8" s="85" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2757,8 +2760,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2781,8 +2784,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
-      <c r="B10" s="79" t="s">
+      <c r="A10" s="87"/>
+      <c r="B10" s="85" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2807,8 +2810,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
-      <c r="B11" s="80"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2831,7 +2834,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="77" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2989,7 +2992,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3015,7 +3018,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="77" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3173,7 +3176,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
+      <c r="A25" s="79"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3199,7 +3202,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="84" t="s">
+      <c r="A26" s="77" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3357,7 +3360,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="85"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3383,7 +3386,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3541,7 +3544,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3567,7 +3570,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="80" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3751,7 +3754,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="84" t="s">
+      <c r="A47" s="77" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3909,7 +3912,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="85"/>
+      <c r="A53" s="79"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3935,7 +3938,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="77" t="s">
+      <c r="A54" s="80" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4119,7 +4122,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="84" t="s">
+      <c r="A61" s="77" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4277,7 +4280,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="85"/>
+      <c r="A67" s="79"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4303,7 +4306,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="84" t="s">
+      <c r="A68" s="77" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4461,7 +4464,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="85"/>
+      <c r="A74" s="79"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4487,7 +4490,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="77" t="s">
+      <c r="A75" s="80" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4645,7 +4648,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="87"/>
+      <c r="A81" s="81"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4672,23 +4675,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4703,7 +4706,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4714,128 +4717,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="95" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="91" t="s">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="90" t="s">
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="91" t="s">
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="90" t="s">
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
+      <c r="AA1" s="88"/>
+      <c r="AB1" s="88"/>
+      <c r="AC1" s="88"/>
+      <c r="AD1" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="90"/>
-      <c r="AJ1" s="91" t="s">
+      <c r="AE1" s="89"/>
+      <c r="AF1" s="89"/>
+      <c r="AG1" s="89"/>
+      <c r="AH1" s="89"/>
+      <c r="AI1" s="89"/>
+      <c r="AJ1" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91"/>
-      <c r="AM1" s="91"/>
-      <c r="AN1" s="91"/>
-      <c r="AO1" s="91"/>
-      <c r="AP1" s="90" t="s">
+      <c r="AK1" s="88"/>
+      <c r="AL1" s="88"/>
+      <c r="AM1" s="88"/>
+      <c r="AN1" s="88"/>
+      <c r="AO1" s="88"/>
+      <c r="AP1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="90"/>
-      <c r="AR1" s="90"/>
-      <c r="AS1" s="90"/>
-      <c r="AT1" s="90"/>
-      <c r="AU1" s="90"/>
-      <c r="AV1" s="91" t="s">
+      <c r="AQ1" s="89"/>
+      <c r="AR1" s="89"/>
+      <c r="AS1" s="89"/>
+      <c r="AT1" s="89"/>
+      <c r="AU1" s="89"/>
+      <c r="AV1" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="91"/>
-      <c r="AX1" s="91"/>
-      <c r="AY1" s="91"/>
-      <c r="AZ1" s="91"/>
-      <c r="BA1" s="91"/>
-      <c r="BB1" s="90" t="s">
+      <c r="AW1" s="88"/>
+      <c r="AX1" s="88"/>
+      <c r="AY1" s="88"/>
+      <c r="AZ1" s="88"/>
+      <c r="BA1" s="88"/>
+      <c r="BB1" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="BC1" s="90"/>
-      <c r="BD1" s="90"/>
-      <c r="BE1" s="90"/>
-      <c r="BF1" s="90"/>
-      <c r="BG1" s="90"/>
-      <c r="BH1" s="91" t="s">
+      <c r="BC1" s="89"/>
+      <c r="BD1" s="89"/>
+      <c r="BE1" s="89"/>
+      <c r="BF1" s="89"/>
+      <c r="BG1" s="89"/>
+      <c r="BH1" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="BI1" s="91"/>
-      <c r="BJ1" s="91"/>
-      <c r="BK1" s="91"/>
-      <c r="BL1" s="91"/>
-      <c r="BM1" s="91"/>
-      <c r="BN1" s="90" t="s">
+      <c r="BI1" s="88"/>
+      <c r="BJ1" s="88"/>
+      <c r="BK1" s="88"/>
+      <c r="BL1" s="88"/>
+      <c r="BM1" s="88"/>
+      <c r="BN1" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="BO1" s="90"/>
-      <c r="BP1" s="90"/>
-      <c r="BQ1" s="90"/>
-      <c r="BR1" s="90"/>
-      <c r="BS1" s="96"/>
+      <c r="BO1" s="89"/>
+      <c r="BP1" s="89"/>
+      <c r="BQ1" s="89"/>
+      <c r="BR1" s="89"/>
+      <c r="BS1" s="90"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="94" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94" t="s">
+      <c r="D2" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="94"/>
+      <c r="K2" s="95"/>
       <c r="L2" s="26" t="s">
         <v>29</v>
       </c>
@@ -5085,7 +5088,7 @@
         <v>0</v>
       </c>
       <c r="W3" s="41">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X3" s="40">
         <v>0</v>
@@ -5103,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="AC3" s="41">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AD3" s="40">
         <v>0</v>
@@ -5300,7 +5303,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X4" s="42">
         <v>0</v>
@@ -5318,16 +5321,16 @@
         <v>0</v>
       </c>
       <c r="AC4" s="43">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AD4" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="30">
         <v>0</v>
       </c>
       <c r="AF4" s="30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="30">
         <v>0</v>
@@ -5342,37 +5345,37 @@
         <v>1</v>
       </c>
       <c r="AK4" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM4" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="30">
         <v>0</v>
       </c>
       <c r="AO4" s="43">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AP4" s="30">
         <v>2</v>
       </c>
       <c r="AQ4" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AR4" s="30">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS4" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AT4" s="30">
         <v>0</v>
       </c>
       <c r="AU4" s="30">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="AV4" s="62">
         <v>0</v>
@@ -5500,7 +5503,7 @@
         <v>5</v>
       </c>
       <c r="R5" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="30">
         <v>0</v>
@@ -5518,7 +5521,7 @@
         <v>10</v>
       </c>
       <c r="X5" s="42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="30">
         <v>0</v>
@@ -5536,7 +5539,7 @@
         <v>20</v>
       </c>
       <c r="AD5" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5" s="30">
         <v>0</v>
@@ -5584,64 +5587,64 @@
         <v>0</v>
       </c>
       <c r="AT5" s="30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AU5" s="30">
         <v>50</v>
       </c>
-      <c r="AV5" s="62">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="63">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="63">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="63">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="64">
-        <v>60</v>
-      </c>
-      <c r="BB5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="63">
-        <v>60</v>
-      </c>
-      <c r="BH5" s="62">
-        <v>0</v>
-      </c>
-      <c r="BI5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="63">
-        <v>0</v>
-      </c>
-      <c r="BM5" s="64">
-        <v>60</v>
+      <c r="AV5" s="73">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="74">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="74">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="74">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="74">
+        <v>10</v>
+      </c>
+      <c r="BA5" s="97">
+        <v>80</v>
+      </c>
+      <c r="BB5" s="74">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="74">
+        <v>10</v>
+      </c>
+      <c r="BG5" s="74">
+        <v>80</v>
+      </c>
+      <c r="BH5" s="73">
+        <v>2</v>
+      </c>
+      <c r="BI5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="74">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="74">
+        <v>10</v>
+      </c>
+      <c r="BM5" s="97">
+        <v>80</v>
       </c>
       <c r="BN5" s="63">
         <v>0</v>
@@ -15769,6 +15772,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L1:Q1"/>
     <mergeCell ref="AV1:BA1"/>
     <mergeCell ref="BB1:BG1"/>
     <mergeCell ref="BH1:BM1"/>
@@ -15785,7 +15789,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:Q1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
tuning level 14 -> 15
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1324,10 +1324,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1337,24 +1355,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="88" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2612,7 +2612,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2638,10 +2638,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="89" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2666,8 +2666,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2690,8 +2690,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="91"/>
+      <c r="B6" s="89" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2716,8 +2716,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="85"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="89"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2740,8 +2740,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
-      <c r="B8" s="83" t="s">
+      <c r="A8" s="91"/>
+      <c r="B8" s="89" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2766,8 +2766,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2790,8 +2790,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
-      <c r="B10" s="83" t="s">
+      <c r="A10" s="91"/>
+      <c r="B10" s="89" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2816,8 +2816,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2840,7 +2840,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="81" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2998,7 +2998,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="81" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3182,7 +3182,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="81" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3366,7 +3366,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="81" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3550,7 +3550,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="84" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3760,7 +3760,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="81" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3918,7 +3918,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="89"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="84" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4128,7 +4128,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88" t="s">
+      <c r="A61" s="81" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4286,7 +4286,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="89"/>
+      <c r="A67" s="83"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4312,7 +4312,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="81" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4470,7 +4470,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="89"/>
+      <c r="A74" s="83"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="81" t="s">
+      <c r="A75" s="84" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4654,7 +4654,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="91"/>
+      <c r="A81" s="85"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4681,23 +4681,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4712,7 +4712,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AT17" sqref="AT17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7822,7 +7822,7 @@
       </c>
     </row>
     <row r="16" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="63">
+      <c r="A16" s="70">
         <v>14</v>
       </c>
       <c r="B16" s="64">
@@ -8037,7 +8037,7 @@
       </c>
     </row>
     <row r="17" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="63">
+      <c r="A17" s="70">
         <v>15</v>
       </c>
       <c r="B17" s="64">
@@ -8050,7 +8050,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="67">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" s="45">
         <v>0</v>
@@ -8164,37 +8164,37 @@
         <v>5</v>
       </c>
       <c r="AQ17" s="67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR17" s="67">
         <v>0</v>
       </c>
       <c r="AS17" s="67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AT17" s="67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AU17" s="67">
-        <v>25</v>
-      </c>
-      <c r="AV17" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW17" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX17" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY17" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ17" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA17" s="57">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="AV17" s="38">
+        <v>7</v>
+      </c>
+      <c r="AW17" s="67">
+        <v>0</v>
+      </c>
+      <c r="AX17" s="67">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="67">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="67">
+        <v>10</v>
+      </c>
+      <c r="BA17" s="39">
+        <v>85</v>
       </c>
       <c r="BB17" s="56">
         <v>0</v>

</xml_diff>

<commit_message>
tuning level 16 a tester
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1324,28 +1324,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1357,16 +1339,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1379,9 +1382,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2612,7 +2612,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
+      <c r="A3" s="90"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2638,10 +2638,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2666,8 +2666,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
-      <c r="B5" s="89"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2690,8 +2690,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
-      <c r="B6" s="89" t="s">
+      <c r="A6" s="85"/>
+      <c r="B6" s="83" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2716,8 +2716,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
-      <c r="B7" s="89"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2740,8 +2740,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="89" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="83" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2766,8 +2766,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2790,8 +2790,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
-      <c r="B10" s="89" t="s">
+      <c r="A10" s="85"/>
+      <c r="B10" s="83" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2816,8 +2816,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
-      <c r="B11" s="90"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2840,7 +2840,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="88" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2998,7 +2998,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
+      <c r="A18" s="89"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="88" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3182,7 +3182,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
+      <c r="A25" s="89"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="88" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3366,7 +3366,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
+      <c r="A32" s="89"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="88" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3550,7 +3550,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
+      <c r="A39" s="89"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="81" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3760,7 +3760,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="88" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3918,7 +3918,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="83"/>
+      <c r="A53" s="89"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="84" t="s">
+      <c r="A54" s="81" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4128,7 +4128,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="88" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4286,7 +4286,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="83"/>
+      <c r="A67" s="89"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4312,7 +4312,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="81" t="s">
+      <c r="A68" s="88" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4470,7 +4470,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="83"/>
+      <c r="A74" s="89"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="84" t="s">
+      <c r="A75" s="81" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4654,7 +4654,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="85"/>
+      <c r="A81" s="91"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4681,23 +4681,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4712,7 +4712,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4723,128 +4723,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="99" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="95" t="s">
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="94" t="s">
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="95" t="s">
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="95"/>
-      <c r="AB1" s="95"/>
-      <c r="AC1" s="95"/>
-      <c r="AD1" s="94" t="s">
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="94"/>
-      <c r="AF1" s="94"/>
-      <c r="AG1" s="94"/>
-      <c r="AH1" s="94"/>
-      <c r="AI1" s="94"/>
-      <c r="AJ1" s="95" t="s">
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="93"/>
+      <c r="AG1" s="93"/>
+      <c r="AH1" s="93"/>
+      <c r="AI1" s="93"/>
+      <c r="AJ1" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="95"/>
-      <c r="AL1" s="95"/>
-      <c r="AM1" s="95"/>
-      <c r="AN1" s="95"/>
-      <c r="AO1" s="95"/>
-      <c r="AP1" s="94" t="s">
+      <c r="AK1" s="92"/>
+      <c r="AL1" s="92"/>
+      <c r="AM1" s="92"/>
+      <c r="AN1" s="92"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" s="94"/>
-      <c r="AR1" s="94"/>
-      <c r="AS1" s="94"/>
-      <c r="AT1" s="94"/>
-      <c r="AU1" s="94"/>
-      <c r="AV1" s="95" t="s">
+      <c r="AQ1" s="93"/>
+      <c r="AR1" s="93"/>
+      <c r="AS1" s="93"/>
+      <c r="AT1" s="93"/>
+      <c r="AU1" s="93"/>
+      <c r="AV1" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="95"/>
-      <c r="AX1" s="95"/>
-      <c r="AY1" s="95"/>
-      <c r="AZ1" s="95"/>
-      <c r="BA1" s="95"/>
-      <c r="BB1" s="94" t="s">
+      <c r="AW1" s="92"/>
+      <c r="AX1" s="92"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="92"/>
+      <c r="BA1" s="92"/>
+      <c r="BB1" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="BC1" s="94"/>
-      <c r="BD1" s="94"/>
-      <c r="BE1" s="94"/>
-      <c r="BF1" s="94"/>
-      <c r="BG1" s="94"/>
-      <c r="BH1" s="95" t="s">
+      <c r="BC1" s="93"/>
+      <c r="BD1" s="93"/>
+      <c r="BE1" s="93"/>
+      <c r="BF1" s="93"/>
+      <c r="BG1" s="93"/>
+      <c r="BH1" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="95"/>
-      <c r="BJ1" s="95"/>
-      <c r="BK1" s="95"/>
-      <c r="BL1" s="95"/>
-      <c r="BM1" s="95"/>
-      <c r="BN1" s="94" t="s">
+      <c r="BI1" s="92"/>
+      <c r="BJ1" s="92"/>
+      <c r="BK1" s="92"/>
+      <c r="BL1" s="92"/>
+      <c r="BM1" s="92"/>
+      <c r="BN1" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="BO1" s="94"/>
-      <c r="BP1" s="94"/>
-      <c r="BQ1" s="94"/>
-      <c r="BR1" s="94"/>
-      <c r="BS1" s="100"/>
+      <c r="BO1" s="93"/>
+      <c r="BP1" s="93"/>
+      <c r="BQ1" s="93"/>
+      <c r="BR1" s="93"/>
+      <c r="BS1" s="94"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="93"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98" t="s">
+      <c r="D2" s="99" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98" t="s">
+      <c r="G2" s="99"/>
+      <c r="H2" s="99" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="98"/>
+      <c r="K2" s="99"/>
       <c r="L2" s="26" t="s">
         <v>28</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="64">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C18" s="65">
         <v>10</v>
@@ -8267,11 +8267,11 @@
       <c r="E18" s="67">
         <v>3</v>
       </c>
-      <c r="F18" s="45">
-        <v>0</v>
-      </c>
-      <c r="G18" s="45">
-        <v>0</v>
+      <c r="F18" s="67">
+        <v>11</v>
+      </c>
+      <c r="G18" s="67">
+        <v>12</v>
       </c>
       <c r="H18" s="67">
         <v>1</v>
@@ -8393,23 +8393,23 @@
       <c r="AU18" s="67">
         <v>25</v>
       </c>
-      <c r="AV18" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW18" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX18" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY18" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA18" s="57">
-        <v>30</v>
+      <c r="AV18" s="38">
+        <v>8</v>
+      </c>
+      <c r="AW18" s="67">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="67">
+        <v>10</v>
+      </c>
+      <c r="AY18" s="67">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="67">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="39">
+        <v>40</v>
       </c>
       <c r="BB18" s="56">
         <v>0</v>
@@ -8477,7 +8477,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="66">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="67">
         <v>28</v>
@@ -15778,6 +15778,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L1:Q1"/>
     <mergeCell ref="AV1:BA1"/>
     <mergeCell ref="BB1:BG1"/>
     <mergeCell ref="BH1:BM1"/>
@@ -15794,7 +15795,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:Q1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
tuning level 16 -> 19
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1270,9 +1270,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1324,10 +1321,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1337,24 +1352,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,6 +1379,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1699,75 +1699,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
+      <c r="AE1" s="79"/>
     </row>
     <row r="2" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="79">
+      <c r="B2" s="78">
         <v>30</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="79"/>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="79"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
     </row>
     <row r="3" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79">
+      <c r="A3" s="78">
         <v>19</v>
       </c>
       <c r="B3" s="3">
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1897,7 +1897,7 @@
       <c r="AE4" s="2"/>
     </row>
     <row r="5" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="AE5" s="2"/>
     </row>
     <row r="6" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1967,7 +1967,7 @@
       <c r="AE6" s="2"/>
     </row>
     <row r="7" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="AE7" s="2"/>
     </row>
     <row r="8" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -2037,7 +2037,7 @@
       <c r="AE8" s="2"/>
     </row>
     <row r="9" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="AE9" s="2"/>
     </row>
     <row r="10" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="AE10" s="2"/>
     </row>
     <row r="11" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="2">
         <v>8</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="AE11" s="2"/>
     </row>
     <row r="12" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="AE12" s="2"/>
     </row>
     <row r="13" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="2">
         <v>10</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="AE13" s="2"/>
     </row>
     <row r="14" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -2247,7 +2247,7 @@
       <c r="AE14" s="2"/>
     </row>
     <row r="15" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="2">
         <v>12</v>
       </c>
@@ -2282,7 +2282,7 @@
       <c r="AE15" s="2"/>
     </row>
     <row r="16" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="2">
         <v>13</v>
       </c>
@@ -2317,7 +2317,7 @@
       <c r="AE16" s="2"/>
     </row>
     <row r="17" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="2">
         <v>14</v>
       </c>
@@ -2352,7 +2352,7 @@
       <c r="AE17" s="2"/>
     </row>
     <row r="18" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="2">
         <v>15</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="AE18" s="2"/>
     </row>
     <row r="19" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
+      <c r="A19" s="78"/>
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="AE19" s="2"/>
     </row>
     <row r="20" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
+      <c r="A20" s="78"/>
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -2457,7 +2457,7 @@
       <c r="AE20" s="2"/>
     </row>
     <row r="21" spans="1:31" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -2518,10 +2518,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="86"/>
       <c r="C1" s="6">
         <v>1</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="87" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2612,7 +2612,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2638,10 +2638,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2666,8 +2666,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2690,8 +2690,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="90"/>
+      <c r="B6" s="88" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2716,8 +2716,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="85"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2740,8 +2740,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
-      <c r="B8" s="83" t="s">
+      <c r="A8" s="90"/>
+      <c r="B8" s="88" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2766,8 +2766,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2790,8 +2790,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
-      <c r="B10" s="83" t="s">
+      <c r="A10" s="90"/>
+      <c r="B10" s="88" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2816,8 +2816,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2840,7 +2840,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="80" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2868,7 +2868,7 @@
       <c r="V12" s="21"/>
     </row>
     <row r="13" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="22" t="s">
         <v>12</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="V13" s="14"/>
     </row>
     <row r="14" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="82"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="V14" s="14"/>
     </row>
     <row r="15" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="22" t="s">
         <v>14</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="V15" s="14"/>
     </row>
     <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="22" t="s">
         <v>15</v>
       </c>
@@ -2972,7 +2972,7 @@
       <c r="V16" s="14"/>
     </row>
     <row r="17" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="82"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="22" t="s">
         <v>16</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="80" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3052,7 +3052,7 @@
       <c r="V19" s="21"/>
     </row>
     <row r="20" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="82"/>
+      <c r="A20" s="81"/>
       <c r="B20" s="22" t="s">
         <v>12</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="V20" s="14"/>
     </row>
     <row r="21" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="82"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="22" t="s">
         <v>13</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="V21" s="14"/>
     </row>
     <row r="22" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="82"/>
+      <c r="A22" s="81"/>
       <c r="B22" s="22" t="s">
         <v>14</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="V22" s="14"/>
     </row>
     <row r="23" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="82"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="22" t="s">
         <v>15</v>
       </c>
@@ -3156,7 +3156,7 @@
       <c r="V23" s="14"/>
     </row>
     <row r="24" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="82"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="22" t="s">
         <v>16</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
+      <c r="A25" s="82"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="80" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3236,7 +3236,7 @@
       <c r="V26" s="21"/>
     </row>
     <row r="27" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="82"/>
+      <c r="A27" s="81"/>
       <c r="B27" s="22" t="s">
         <v>12</v>
       </c>
@@ -3262,7 +3262,7 @@
       <c r="V27" s="14"/>
     </row>
     <row r="28" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="82"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="22" t="s">
         <v>13</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="V28" s="14"/>
     </row>
     <row r="29" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="22" t="s">
         <v>14</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="V29" s="14"/>
     </row>
     <row r="30" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="22" t="s">
         <v>15</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="V30" s="14"/>
     </row>
     <row r="31" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="82"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="22" t="s">
         <v>16</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
+      <c r="A32" s="82"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="80" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3420,7 +3420,7 @@
       <c r="V33" s="21"/>
     </row>
     <row r="34" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="82"/>
+      <c r="A34" s="81"/>
       <c r="B34" s="22" t="s">
         <v>12</v>
       </c>
@@ -3446,7 +3446,7 @@
       <c r="V34" s="14"/>
     </row>
     <row r="35" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="22" t="s">
         <v>13</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="V35" s="14"/>
     </row>
     <row r="36" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="82"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="22" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="V36" s="14"/>
     </row>
     <row r="37" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="22" t="s">
         <v>15</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="V37" s="14"/>
     </row>
     <row r="38" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="82"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="22" t="s">
         <v>16</v>
       </c>
@@ -3550,7 +3550,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
+      <c r="A39" s="82"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="83" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3604,7 +3604,7 @@
       <c r="V40" s="21"/>
     </row>
     <row r="41" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="82"/>
+      <c r="A41" s="81"/>
       <c r="B41" s="22" t="s">
         <v>12</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="V41" s="14"/>
     </row>
     <row r="42" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="82"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="22" t="s">
         <v>13</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="V42" s="14"/>
     </row>
     <row r="43" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="82"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="22" t="s">
         <v>14</v>
       </c>
@@ -3682,7 +3682,7 @@
       <c r="V43" s="14"/>
     </row>
     <row r="44" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="82"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="22" t="s">
         <v>15</v>
       </c>
@@ -3708,7 +3708,7 @@
       <c r="V44" s="14"/>
     </row>
     <row r="45" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="82"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="22" t="s">
         <v>16</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="V45" s="14"/>
     </row>
     <row r="46" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="82"/>
+      <c r="A46" s="81"/>
       <c r="B46" s="23" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="80" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3788,7 +3788,7 @@
       <c r="V47" s="21"/>
     </row>
     <row r="48" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="82"/>
+      <c r="A48" s="81"/>
       <c r="B48" s="22" t="s">
         <v>12</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="V48" s="14"/>
     </row>
     <row r="49" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="82"/>
+      <c r="A49" s="81"/>
       <c r="B49" s="22" t="s">
         <v>13</v>
       </c>
@@ -3840,7 +3840,7 @@
       <c r="V49" s="14"/>
     </row>
     <row r="50" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="82"/>
+      <c r="A50" s="81"/>
       <c r="B50" s="22" t="s">
         <v>14</v>
       </c>
@@ -3866,7 +3866,7 @@
       <c r="V50" s="14"/>
     </row>
     <row r="51" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="82"/>
+      <c r="A51" s="81"/>
       <c r="B51" s="22" t="s">
         <v>15</v>
       </c>
@@ -3892,7 +3892,7 @@
       <c r="V51" s="14"/>
     </row>
     <row r="52" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="82"/>
+      <c r="A52" s="81"/>
       <c r="B52" s="22" t="s">
         <v>16</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="89"/>
+      <c r="A53" s="82"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="83" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -3972,7 +3972,7 @@
       <c r="V54" s="21"/>
     </row>
     <row r="55" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="82"/>
+      <c r="A55" s="81"/>
       <c r="B55" s="22" t="s">
         <v>12</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="V55" s="14"/>
     </row>
     <row r="56" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="82"/>
+      <c r="A56" s="81"/>
       <c r="B56" s="22" t="s">
         <v>13</v>
       </c>
@@ -4024,7 +4024,7 @@
       <c r="V56" s="14"/>
     </row>
     <row r="57" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="82"/>
+      <c r="A57" s="81"/>
       <c r="B57" s="22" t="s">
         <v>14</v>
       </c>
@@ -4050,7 +4050,7 @@
       <c r="V57" s="14"/>
     </row>
     <row r="58" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="82"/>
+      <c r="A58" s="81"/>
       <c r="B58" s="22" t="s">
         <v>15</v>
       </c>
@@ -4076,7 +4076,7 @@
       <c r="V58" s="14"/>
     </row>
     <row r="59" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="82"/>
+      <c r="A59" s="81"/>
       <c r="B59" s="22" t="s">
         <v>16</v>
       </c>
@@ -4102,7 +4102,7 @@
       <c r="V59" s="14"/>
     </row>
     <row r="60" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="82"/>
+      <c r="A60" s="81"/>
       <c r="B60" s="23" t="s">
         <v>17</v>
       </c>
@@ -4128,7 +4128,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88" t="s">
+      <c r="A61" s="80" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4156,7 +4156,7 @@
       <c r="V61" s="21"/>
     </row>
     <row r="62" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="82"/>
+      <c r="A62" s="81"/>
       <c r="B62" s="22" t="s">
         <v>12</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="V62" s="14"/>
     </row>
     <row r="63" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="82"/>
+      <c r="A63" s="81"/>
       <c r="B63" s="22" t="s">
         <v>13</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="V63" s="14"/>
     </row>
     <row r="64" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="82"/>
+      <c r="A64" s="81"/>
       <c r="B64" s="22" t="s">
         <v>14</v>
       </c>
@@ -4234,7 +4234,7 @@
       <c r="V64" s="14"/>
     </row>
     <row r="65" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="82"/>
+      <c r="A65" s="81"/>
       <c r="B65" s="22" t="s">
         <v>15</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="V65" s="14"/>
     </row>
     <row r="66" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="82"/>
+      <c r="A66" s="81"/>
       <c r="B66" s="22" t="s">
         <v>16</v>
       </c>
@@ -4286,7 +4286,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="89"/>
+      <c r="A67" s="82"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4312,7 +4312,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="80" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4340,7 +4340,7 @@
       <c r="V68" s="21"/>
     </row>
     <row r="69" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="82"/>
+      <c r="A69" s="81"/>
       <c r="B69" s="22" t="s">
         <v>12</v>
       </c>
@@ -4366,7 +4366,7 @@
       <c r="V69" s="14"/>
     </row>
     <row r="70" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="82"/>
+      <c r="A70" s="81"/>
       <c r="B70" s="22" t="s">
         <v>13</v>
       </c>
@@ -4392,7 +4392,7 @@
       <c r="V70" s="14"/>
     </row>
     <row r="71" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="82"/>
+      <c r="A71" s="81"/>
       <c r="B71" s="22" t="s">
         <v>14</v>
       </c>
@@ -4418,7 +4418,7 @@
       <c r="V71" s="14"/>
     </row>
     <row r="72" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="82"/>
+      <c r="A72" s="81"/>
       <c r="B72" s="22" t="s">
         <v>15</v>
       </c>
@@ -4444,7 +4444,7 @@
       <c r="V72" s="14"/>
     </row>
     <row r="73" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="82"/>
+      <c r="A73" s="81"/>
       <c r="B73" s="22" t="s">
         <v>16</v>
       </c>
@@ -4470,7 +4470,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="89"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="81" t="s">
+      <c r="A75" s="83" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4524,7 +4524,7 @@
       <c r="V75" s="21"/>
     </row>
     <row r="76" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="82"/>
+      <c r="A76" s="81"/>
       <c r="B76" s="22" t="s">
         <v>12</v>
       </c>
@@ -4550,7 +4550,7 @@
       <c r="V76" s="14"/>
     </row>
     <row r="77" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="82"/>
+      <c r="A77" s="81"/>
       <c r="B77" s="22" t="s">
         <v>13</v>
       </c>
@@ -4576,7 +4576,7 @@
       <c r="V77" s="14"/>
     </row>
     <row r="78" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="82"/>
+      <c r="A78" s="81"/>
       <c r="B78" s="22" t="s">
         <v>14</v>
       </c>
@@ -4602,7 +4602,7 @@
       <c r="V78" s="14"/>
     </row>
     <row r="79" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="82"/>
+      <c r="A79" s="81"/>
       <c r="B79" s="22" t="s">
         <v>15</v>
       </c>
@@ -4628,7 +4628,7 @@
       <c r="V79" s="14"/>
     </row>
     <row r="80" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="82"/>
+      <c r="A80" s="81"/>
       <c r="B80" s="22" t="s">
         <v>16</v>
       </c>
@@ -4654,7 +4654,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="91"/>
+      <c r="A81" s="84"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4681,23 +4681,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4712,7 +4712,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+      <selection activeCell="AZ21" sqref="AZ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4723,128 +4723,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="100" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="92" t="s">
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="93" t="s">
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-      <c r="X1" s="92" t="s">
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="92"/>
-      <c r="Z1" s="92"/>
-      <c r="AA1" s="92"/>
-      <c r="AB1" s="92"/>
-      <c r="AC1" s="92"/>
-      <c r="AD1" s="93" t="s">
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93"/>
-      <c r="AJ1" s="92" t="s">
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="92"/>
-      <c r="AL1" s="92"/>
-      <c r="AM1" s="92"/>
-      <c r="AN1" s="92"/>
-      <c r="AO1" s="92"/>
-      <c r="AP1" s="93" t="s">
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" s="93"/>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
-      <c r="AU1" s="93"/>
-      <c r="AV1" s="92" t="s">
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="92"/>
-      <c r="AX1" s="92"/>
-      <c r="AY1" s="92"/>
-      <c r="AZ1" s="92"/>
-      <c r="BA1" s="92"/>
-      <c r="BB1" s="93" t="s">
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="91"/>
+      <c r="AY1" s="91"/>
+      <c r="AZ1" s="91"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="BC1" s="93"/>
-      <c r="BD1" s="93"/>
-      <c r="BE1" s="93"/>
-      <c r="BF1" s="93"/>
-      <c r="BG1" s="93"/>
-      <c r="BH1" s="92" t="s">
+      <c r="BC1" s="92"/>
+      <c r="BD1" s="92"/>
+      <c r="BE1" s="92"/>
+      <c r="BF1" s="92"/>
+      <c r="BG1" s="92"/>
+      <c r="BH1" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="92"/>
-      <c r="BJ1" s="92"/>
-      <c r="BK1" s="92"/>
-      <c r="BL1" s="92"/>
-      <c r="BM1" s="92"/>
-      <c r="BN1" s="93" t="s">
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="91"/>
+      <c r="BK1" s="91"/>
+      <c r="BL1" s="91"/>
+      <c r="BM1" s="91"/>
+      <c r="BN1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="BO1" s="93"/>
-      <c r="BP1" s="93"/>
-      <c r="BQ1" s="93"/>
-      <c r="BR1" s="93"/>
-      <c r="BS1" s="94"/>
+      <c r="BO1" s="92"/>
+      <c r="BP1" s="92"/>
+      <c r="BQ1" s="92"/>
+      <c r="BR1" s="92"/>
+      <c r="BS1" s="93"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96"/>
+      <c r="A2" s="95"/>
       <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="99" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99" t="s">
+      <c r="D2" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99" t="s">
+      <c r="G2" s="98"/>
+      <c r="H2" s="98" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="99"/>
+      <c r="K2" s="98"/>
       <c r="L2" s="26" t="s">
         <v>28</v>
       </c>
@@ -5027,7 +5027,7 @@
       </c>
     </row>
     <row r="3" spans="1:71" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69">
+      <c r="A3" s="68">
         <v>1</v>
       </c>
       <c r="B3" s="31">
@@ -5242,7 +5242,7 @@
       </c>
     </row>
     <row r="4" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70">
+      <c r="A4" s="69">
         <v>2</v>
       </c>
       <c r="B4" s="32">
@@ -5457,7 +5457,7 @@
       </c>
     </row>
     <row r="5" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
+      <c r="A5" s="70">
         <v>3</v>
       </c>
       <c r="B5" s="32">
@@ -5598,58 +5598,58 @@
       <c r="AU5" s="30">
         <v>50</v>
       </c>
-      <c r="AV5" s="66">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="67">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="67">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="67">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="67">
-        <v>10</v>
-      </c>
-      <c r="BA5" s="68">
+      <c r="AV5" s="65">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="66">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="66">
+        <v>10</v>
+      </c>
+      <c r="BA5" s="67">
         <v>80</v>
       </c>
-      <c r="BB5" s="67">
+      <c r="BB5" s="66">
         <v>1</v>
       </c>
-      <c r="BC5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="67">
-        <v>10</v>
-      </c>
-      <c r="BG5" s="67">
+      <c r="BC5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="66">
+        <v>10</v>
+      </c>
+      <c r="BG5" s="66">
         <v>80</v>
       </c>
-      <c r="BH5" s="66">
+      <c r="BH5" s="65">
         <v>2</v>
       </c>
-      <c r="BI5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="67">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="67">
-        <v>10</v>
-      </c>
-      <c r="BM5" s="68">
+      <c r="BI5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="66">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="66">
+        <v>10</v>
+      </c>
+      <c r="BM5" s="67">
         <v>80</v>
       </c>
       <c r="BN5" s="56">
@@ -5672,7 +5672,7 @@
       </c>
     </row>
     <row r="6" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70">
+      <c r="A6" s="69">
         <v>4</v>
       </c>
       <c r="B6" s="32">
@@ -5795,40 +5795,40 @@
       <c r="AO6" s="39">
         <v>85</v>
       </c>
-      <c r="AP6" s="67">
+      <c r="AP6" s="66">
         <v>2</v>
       </c>
-      <c r="AQ6" s="67">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="67">
-        <v>10</v>
-      </c>
-      <c r="AU6" s="67">
+      <c r="AQ6" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="66">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="66">
+        <v>10</v>
+      </c>
+      <c r="AU6" s="66">
         <v>100</v>
       </c>
-      <c r="AV6" s="66">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="67">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="67">
+      <c r="AV6" s="65">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="66">
         <v>20</v>
       </c>
-      <c r="AY6" s="67">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="67">
+      <c r="AY6" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="66">
         <v>20</v>
       </c>
-      <c r="BA6" s="68">
+      <c r="BA6" s="67">
         <v>125</v>
       </c>
       <c r="BB6" s="56">
@@ -5887,7 +5887,7 @@
       </c>
     </row>
     <row r="7" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70">
+      <c r="A7" s="69">
         <v>5</v>
       </c>
       <c r="B7" s="32">
@@ -6064,22 +6064,22 @@
       <c r="BG7" s="30">
         <v>95</v>
       </c>
-      <c r="BH7" s="66">
+      <c r="BH7" s="65">
         <v>2</v>
       </c>
-      <c r="BI7" s="67">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="67">
-        <v>0</v>
-      </c>
-      <c r="BK7" s="67">
-        <v>10</v>
-      </c>
-      <c r="BL7" s="67">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="68">
+      <c r="BI7" s="66">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="66">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="66">
+        <v>10</v>
+      </c>
+      <c r="BL7" s="66">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="67">
         <v>100</v>
       </c>
       <c r="BN7" s="56">
@@ -6102,7 +6102,7 @@
       </c>
     </row>
     <row r="8" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="70">
+      <c r="A8" s="69">
         <v>6</v>
       </c>
       <c r="B8" s="32">
@@ -6317,7 +6317,7 @@
       </c>
     </row>
     <row r="9" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70">
+      <c r="A9" s="69">
         <v>7</v>
       </c>
       <c r="B9" s="32">
@@ -6532,7 +6532,7 @@
       </c>
     </row>
     <row r="10" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70">
+      <c r="A10" s="69">
         <v>8</v>
       </c>
       <c r="B10" s="32">
@@ -6747,7 +6747,7 @@
       </c>
     </row>
     <row r="11" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70">
+      <c r="A11" s="69">
         <v>9</v>
       </c>
       <c r="B11" s="32">
@@ -6962,7 +6962,7 @@
       </c>
     </row>
     <row r="12" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70">
+      <c r="A12" s="69">
         <v>10</v>
       </c>
       <c r="B12" s="32">
@@ -7177,37 +7177,37 @@
       </c>
     </row>
     <row r="13" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77">
+      <c r="A13" s="76">
         <v>11</v>
       </c>
-      <c r="B13" s="64">
+      <c r="B13" s="63">
         <v>15</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C13" s="64">
         <v>9</v>
       </c>
-      <c r="D13" s="66">
+      <c r="D13" s="65">
         <v>15</v>
       </c>
-      <c r="E13" s="67">
+      <c r="E13" s="66">
         <v>28</v>
       </c>
-      <c r="F13" s="67">
+      <c r="F13" s="66">
         <v>2</v>
       </c>
-      <c r="G13" s="67">
+      <c r="G13" s="66">
         <v>16</v>
       </c>
-      <c r="H13" s="67">
+      <c r="H13" s="66">
         <v>2</v>
       </c>
-      <c r="I13" s="67">
+      <c r="I13" s="66">
         <v>28</v>
       </c>
-      <c r="J13" s="67">
+      <c r="J13" s="66">
         <v>2</v>
       </c>
-      <c r="K13" s="65">
+      <c r="K13" s="64">
         <v>16</v>
       </c>
       <c r="L13" s="38">
@@ -7392,25 +7392,25 @@
       </c>
     </row>
     <row r="14" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+      <c r="A14" s="76">
         <v>12</v>
       </c>
-      <c r="B14" s="64">
-        <v>3</v>
-      </c>
-      <c r="C14" s="65">
+      <c r="B14" s="63">
+        <v>3</v>
+      </c>
+      <c r="C14" s="64">
         <v>11</v>
       </c>
-      <c r="D14" s="66">
-        <v>5</v>
-      </c>
-      <c r="E14" s="67">
+      <c r="D14" s="65">
+        <v>5</v>
+      </c>
+      <c r="E14" s="66">
         <v>25</v>
       </c>
-      <c r="F14" s="67">
-        <v>3</v>
-      </c>
-      <c r="G14" s="67">
+      <c r="F14" s="66">
+        <v>3</v>
+      </c>
+      <c r="G14" s="66">
         <v>15</v>
       </c>
       <c r="H14" s="45">
@@ -7425,127 +7425,127 @@
       <c r="K14" s="43">
         <v>0</v>
       </c>
-      <c r="L14" s="66">
-        <v>3</v>
-      </c>
-      <c r="M14" s="67">
-        <v>0</v>
-      </c>
-      <c r="N14" s="67">
+      <c r="L14" s="65">
+        <v>3</v>
+      </c>
+      <c r="M14" s="66">
+        <v>0</v>
+      </c>
+      <c r="N14" s="66">
         <v>15</v>
       </c>
-      <c r="O14" s="67">
-        <v>0</v>
-      </c>
-      <c r="P14" s="67">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="68">
-        <v>10</v>
-      </c>
-      <c r="R14" s="78">
-        <v>3</v>
-      </c>
-      <c r="S14" s="67">
-        <v>0</v>
-      </c>
-      <c r="T14" s="67">
+      <c r="O14" s="66">
+        <v>0</v>
+      </c>
+      <c r="P14" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="67">
+        <v>10</v>
+      </c>
+      <c r="R14" s="77">
+        <v>3</v>
+      </c>
+      <c r="S14" s="66">
+        <v>0</v>
+      </c>
+      <c r="T14" s="66">
         <v>15</v>
       </c>
-      <c r="U14" s="67">
-        <v>0</v>
-      </c>
-      <c r="V14" s="67">
-        <v>0</v>
-      </c>
-      <c r="W14" s="67">
-        <v>10</v>
-      </c>
-      <c r="X14" s="66">
-        <v>3</v>
-      </c>
-      <c r="Y14" s="67">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="67">
+      <c r="U14" s="66">
+        <v>0</v>
+      </c>
+      <c r="V14" s="66">
+        <v>0</v>
+      </c>
+      <c r="W14" s="66">
+        <v>10</v>
+      </c>
+      <c r="X14" s="65">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="66">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="66">
         <v>15</v>
       </c>
-      <c r="AA14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD14" s="78">
-        <v>5</v>
-      </c>
-      <c r="AE14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="67">
+      <c r="AA14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="67">
+        <v>10</v>
+      </c>
+      <c r="AD14" s="77">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="66">
         <v>15</v>
       </c>
-      <c r="AG14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="67">
+      <c r="AG14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="66">
         <v>30</v>
       </c>
-      <c r="AJ14" s="66">
+      <c r="AJ14" s="65">
         <v>4</v>
       </c>
-      <c r="AK14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="67">
+      <c r="AK14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="66">
         <v>15</v>
       </c>
-      <c r="AM14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="68">
+      <c r="AM14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="67">
         <v>30</v>
       </c>
-      <c r="AP14" s="67">
+      <c r="AP14" s="66">
         <v>7</v>
       </c>
-      <c r="AQ14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="67">
+      <c r="AQ14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="66">
         <v>1</v>
       </c>
-      <c r="AS14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="67">
+      <c r="AS14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="66">
         <v>70</v>
       </c>
       <c r="AV14" s="38">
         <v>7</v>
       </c>
-      <c r="AW14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="67">
-        <v>10</v>
-      </c>
-      <c r="AY14" s="67">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="67">
+      <c r="AW14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="66">
+        <v>10</v>
+      </c>
+      <c r="AY14" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ14" s="66">
         <v>0</v>
       </c>
       <c r="BA14" s="39">
@@ -7607,13 +7607,13 @@
       </c>
     </row>
     <row r="15" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="70">
+      <c r="A15" s="69">
         <v>13</v>
       </c>
-      <c r="B15" s="64">
+      <c r="B15" s="63">
         <v>15</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="64">
         <v>3</v>
       </c>
       <c r="D15" s="44">
@@ -7622,130 +7622,130 @@
       <c r="E15" s="45">
         <v>0</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="66">
         <v>15</v>
       </c>
-      <c r="G15" s="67">
+      <c r="G15" s="66">
         <v>16</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="66">
         <v>15</v>
       </c>
-      <c r="I15" s="67">
+      <c r="I15" s="66">
         <v>16</v>
       </c>
-      <c r="J15" s="67">
+      <c r="J15" s="66">
         <v>14</v>
       </c>
-      <c r="K15" s="65">
+      <c r="K15" s="64">
         <v>16</v>
       </c>
-      <c r="L15" s="66">
-        <v>0</v>
-      </c>
-      <c r="M15" s="67">
-        <v>0</v>
-      </c>
-      <c r="N15" s="67">
-        <v>5</v>
-      </c>
-      <c r="O15" s="67">
-        <v>5</v>
-      </c>
-      <c r="P15" s="67">
-        <v>5</v>
-      </c>
-      <c r="Q15" s="68">
-        <v>10</v>
-      </c>
-      <c r="R15" s="78">
+      <c r="L15" s="65">
+        <v>0</v>
+      </c>
+      <c r="M15" s="66">
+        <v>0</v>
+      </c>
+      <c r="N15" s="66">
+        <v>5</v>
+      </c>
+      <c r="O15" s="66">
+        <v>5</v>
+      </c>
+      <c r="P15" s="66">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="67">
+        <v>10</v>
+      </c>
+      <c r="R15" s="77">
         <v>1</v>
       </c>
-      <c r="S15" s="67">
-        <v>0</v>
-      </c>
-      <c r="T15" s="67">
-        <v>5</v>
-      </c>
-      <c r="U15" s="67">
-        <v>5</v>
-      </c>
-      <c r="V15" s="67">
-        <v>5</v>
-      </c>
-      <c r="W15" s="67">
+      <c r="S15" s="66">
+        <v>0</v>
+      </c>
+      <c r="T15" s="66">
+        <v>5</v>
+      </c>
+      <c r="U15" s="66">
+        <v>5</v>
+      </c>
+      <c r="V15" s="66">
+        <v>5</v>
+      </c>
+      <c r="W15" s="66">
         <v>15</v>
       </c>
-      <c r="X15" s="66">
+      <c r="X15" s="65">
         <v>2</v>
       </c>
-      <c r="Y15" s="67">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AA15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AB15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AC15" s="68">
+      <c r="Y15" s="66">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AA15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AC15" s="67">
         <v>20</v>
       </c>
-      <c r="AD15" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE15" s="67">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AG15" s="67">
-        <v>10</v>
-      </c>
-      <c r="AH15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AI15" s="67">
+      <c r="AD15" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="66">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AG15" s="66">
+        <v>10</v>
+      </c>
+      <c r="AH15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AI15" s="66">
         <v>25</v>
       </c>
-      <c r="AJ15" s="66">
+      <c r="AJ15" s="65">
         <v>4</v>
       </c>
-      <c r="AK15" s="67">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AM15" s="67">
-        <v>10</v>
-      </c>
-      <c r="AN15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AO15" s="68">
+      <c r="AK15" s="66">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AM15" s="66">
+        <v>10</v>
+      </c>
+      <c r="AN15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AO15" s="67">
         <v>30</v>
       </c>
-      <c r="AP15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ15" s="67">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AS15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AT15" s="67">
-        <v>5</v>
-      </c>
-      <c r="AU15" s="67">
+      <c r="AP15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AQ15" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AS15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AT15" s="66">
+        <v>5</v>
+      </c>
+      <c r="AU15" s="66">
         <v>35</v>
       </c>
       <c r="AV15" s="55">
@@ -7822,145 +7822,145 @@
       </c>
     </row>
     <row r="16" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70">
+      <c r="A16" s="69">
         <v>14</v>
       </c>
-      <c r="B16" s="64">
+      <c r="B16" s="63">
         <v>15</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="64">
         <v>6</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="65">
         <v>2</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="66">
         <v>28</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="66">
         <v>11</v>
       </c>
-      <c r="G16" s="67">
+      <c r="G16" s="66">
         <v>12</v>
       </c>
-      <c r="H16" s="67">
+      <c r="H16" s="66">
         <v>2</v>
       </c>
-      <c r="I16" s="67">
+      <c r="I16" s="66">
         <v>28</v>
       </c>
-      <c r="J16" s="67">
+      <c r="J16" s="66">
         <v>11</v>
       </c>
-      <c r="K16" s="65">
+      <c r="K16" s="64">
         <v>12</v>
       </c>
-      <c r="L16" s="66">
-        <v>0</v>
-      </c>
-      <c r="M16" s="67">
-        <v>0</v>
-      </c>
-      <c r="N16" s="67">
-        <v>10</v>
-      </c>
-      <c r="O16" s="67">
-        <v>0</v>
-      </c>
-      <c r="P16" s="67">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="68">
-        <v>10</v>
-      </c>
-      <c r="R16" s="78">
+      <c r="L16" s="65">
+        <v>0</v>
+      </c>
+      <c r="M16" s="66">
+        <v>0</v>
+      </c>
+      <c r="N16" s="66">
+        <v>10</v>
+      </c>
+      <c r="O16" s="66">
+        <v>0</v>
+      </c>
+      <c r="P16" s="66">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="67">
+        <v>10</v>
+      </c>
+      <c r="R16" s="77">
         <v>1</v>
       </c>
-      <c r="S16" s="67">
-        <v>0</v>
-      </c>
-      <c r="T16" s="67">
-        <v>5</v>
-      </c>
-      <c r="U16" s="67">
-        <v>0</v>
-      </c>
-      <c r="V16" s="67">
-        <v>5</v>
-      </c>
-      <c r="W16" s="67">
+      <c r="S16" s="66">
+        <v>0</v>
+      </c>
+      <c r="T16" s="66">
+        <v>5</v>
+      </c>
+      <c r="U16" s="66">
+        <v>0</v>
+      </c>
+      <c r="V16" s="66">
+        <v>5</v>
+      </c>
+      <c r="W16" s="66">
         <v>20</v>
       </c>
-      <c r="X16" s="66">
+      <c r="X16" s="65">
         <v>2</v>
       </c>
-      <c r="Y16" s="67">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="67">
-        <v>5</v>
-      </c>
-      <c r="AA16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="67">
-        <v>5</v>
-      </c>
-      <c r="AC16" s="68">
+      <c r="Y16" s="66">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="66">
+        <v>5</v>
+      </c>
+      <c r="AA16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="66">
+        <v>5</v>
+      </c>
+      <c r="AC16" s="67">
         <v>30</v>
       </c>
-      <c r="AD16" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE16" s="67">
-        <v>10</v>
-      </c>
-      <c r="AF16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="67">
-        <v>10</v>
-      </c>
-      <c r="AH16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="67">
+      <c r="AD16" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE16" s="66">
+        <v>10</v>
+      </c>
+      <c r="AF16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="66">
+        <v>10</v>
+      </c>
+      <c r="AH16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="66">
         <v>45</v>
       </c>
-      <c r="AJ16" s="66">
-        <v>5</v>
-      </c>
-      <c r="AK16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="67">
-        <v>5</v>
-      </c>
-      <c r="AM16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AN16" s="67">
-        <v>5</v>
-      </c>
-      <c r="AO16" s="68">
+      <c r="AJ16" s="65">
+        <v>5</v>
+      </c>
+      <c r="AK16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="66">
+        <v>5</v>
+      </c>
+      <c r="AM16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="66">
+        <v>5</v>
+      </c>
+      <c r="AO16" s="67">
         <v>65</v>
       </c>
-      <c r="AP16" s="67">
+      <c r="AP16" s="66">
         <v>4</v>
       </c>
-      <c r="AQ16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="67">
+      <c r="AQ16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="66">
         <v>15</v>
       </c>
-      <c r="AS16" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT16" s="67">
+      <c r="AS16" s="66">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="66">
         <v>15</v>
       </c>
-      <c r="AU16" s="67">
+      <c r="AU16" s="66">
         <v>75</v>
       </c>
       <c r="AV16" s="55">
@@ -8037,19 +8037,19 @@
       </c>
     </row>
     <row r="17" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70">
+      <c r="A17" s="69">
         <v>15</v>
       </c>
-      <c r="B17" s="64">
+      <c r="B17" s="63">
         <v>28</v>
       </c>
-      <c r="C17" s="65">
-        <v>10</v>
-      </c>
-      <c r="D17" s="66">
-        <v>5</v>
-      </c>
-      <c r="E17" s="67">
+      <c r="C17" s="64">
+        <v>10</v>
+      </c>
+      <c r="D17" s="65">
+        <v>5</v>
+      </c>
+      <c r="E17" s="66">
         <v>23</v>
       </c>
       <c r="F17" s="45">
@@ -8058,139 +8058,139 @@
       <c r="G17" s="45">
         <v>0</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="66">
         <v>8</v>
       </c>
-      <c r="I17" s="67">
+      <c r="I17" s="66">
         <v>15</v>
       </c>
-      <c r="J17" s="67">
+      <c r="J17" s="66">
         <v>9</v>
       </c>
-      <c r="K17" s="65">
+      <c r="K17" s="64">
         <v>12</v>
       </c>
-      <c r="L17" s="66">
-        <v>0</v>
-      </c>
-      <c r="M17" s="67">
-        <v>3</v>
-      </c>
-      <c r="N17" s="67">
-        <v>0</v>
-      </c>
-      <c r="O17" s="67">
-        <v>3</v>
-      </c>
-      <c r="P17" s="67">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="68">
-        <v>0</v>
-      </c>
-      <c r="R17" s="78">
+      <c r="L17" s="65">
+        <v>0</v>
+      </c>
+      <c r="M17" s="66">
+        <v>3</v>
+      </c>
+      <c r="N17" s="66">
+        <v>0</v>
+      </c>
+      <c r="O17" s="66">
+        <v>3</v>
+      </c>
+      <c r="P17" s="66">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="67">
+        <v>0</v>
+      </c>
+      <c r="R17" s="77">
         <v>1</v>
       </c>
-      <c r="S17" s="67">
-        <v>3</v>
-      </c>
-      <c r="T17" s="67">
-        <v>0</v>
-      </c>
-      <c r="U17" s="67">
-        <v>3</v>
-      </c>
-      <c r="V17" s="67">
-        <v>3</v>
-      </c>
-      <c r="W17" s="67">
-        <v>5</v>
-      </c>
-      <c r="X17" s="66">
+      <c r="S17" s="66">
+        <v>3</v>
+      </c>
+      <c r="T17" s="66">
+        <v>0</v>
+      </c>
+      <c r="U17" s="66">
+        <v>3</v>
+      </c>
+      <c r="V17" s="66">
+        <v>3</v>
+      </c>
+      <c r="W17" s="66">
+        <v>5</v>
+      </c>
+      <c r="X17" s="65">
         <v>2</v>
       </c>
-      <c r="Y17" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AB17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AC17" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AH17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AI17" s="67">
+      <c r="Y17" s="66">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="67">
+        <v>10</v>
+      </c>
+      <c r="AD17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AH17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AI17" s="66">
         <v>15</v>
       </c>
-      <c r="AJ17" s="66">
+      <c r="AJ17" s="65">
         <v>4</v>
       </c>
-      <c r="AK17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AL17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AN17" s="67">
-        <v>3</v>
-      </c>
-      <c r="AO17" s="68">
+      <c r="AK17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="66">
+        <v>3</v>
+      </c>
+      <c r="AO17" s="67">
         <v>50</v>
       </c>
-      <c r="AP17" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ17" s="67">
-        <v>5</v>
-      </c>
-      <c r="AR17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="67">
-        <v>5</v>
-      </c>
-      <c r="AT17" s="67">
-        <v>5</v>
-      </c>
-      <c r="AU17" s="67">
+      <c r="AP17" s="66">
+        <v>5</v>
+      </c>
+      <c r="AQ17" s="66">
+        <v>5</v>
+      </c>
+      <c r="AR17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="66">
+        <v>5</v>
+      </c>
+      <c r="AT17" s="66">
+        <v>5</v>
+      </c>
+      <c r="AU17" s="66">
         <v>60</v>
       </c>
       <c r="AV17" s="38">
         <v>7</v>
       </c>
-      <c r="AW17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AX17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AY17" s="67">
-        <v>0</v>
-      </c>
-      <c r="AZ17" s="67">
+      <c r="AW17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="66">
         <v>10</v>
       </c>
       <c r="BA17" s="39">
@@ -8252,31 +8252,31 @@
       </c>
     </row>
     <row r="18" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63">
+      <c r="A18" s="69">
         <v>16</v>
       </c>
-      <c r="B18" s="64">
+      <c r="B18" s="63">
         <v>14</v>
       </c>
-      <c r="C18" s="65">
-        <v>10</v>
-      </c>
-      <c r="D18" s="66">
+      <c r="C18" s="64">
+        <v>10</v>
+      </c>
+      <c r="D18" s="65">
         <v>2</v>
       </c>
-      <c r="E18" s="67">
-        <v>3</v>
-      </c>
-      <c r="F18" s="67">
-        <v>11</v>
-      </c>
-      <c r="G18" s="67">
-        <v>12</v>
-      </c>
-      <c r="H18" s="67">
+      <c r="E18" s="66">
+        <v>3</v>
+      </c>
+      <c r="F18" s="66">
+        <v>8</v>
+      </c>
+      <c r="G18" s="66">
+        <v>16</v>
+      </c>
+      <c r="H18" s="66">
         <v>1</v>
       </c>
-      <c r="I18" s="67">
+      <c r="I18" s="66">
         <v>8</v>
       </c>
       <c r="J18" s="45">
@@ -8285,149 +8285,149 @@
       <c r="K18" s="43">
         <v>0</v>
       </c>
-      <c r="L18" s="66">
-        <v>0</v>
-      </c>
-      <c r="M18" s="67">
-        <v>3</v>
-      </c>
-      <c r="N18" s="67">
-        <v>0</v>
-      </c>
-      <c r="O18" s="67">
-        <v>3</v>
-      </c>
-      <c r="P18" s="67">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="68">
-        <v>0</v>
-      </c>
-      <c r="R18" s="78">
+      <c r="L18" s="65">
+        <v>0</v>
+      </c>
+      <c r="M18" s="66">
+        <v>5</v>
+      </c>
+      <c r="N18" s="66">
+        <v>0</v>
+      </c>
+      <c r="O18" s="66">
+        <v>5</v>
+      </c>
+      <c r="P18" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="67">
+        <v>5</v>
+      </c>
+      <c r="R18" s="77">
         <v>1</v>
       </c>
-      <c r="S18" s="67">
-        <v>3</v>
-      </c>
-      <c r="T18" s="67">
-        <v>0</v>
-      </c>
-      <c r="U18" s="67">
-        <v>3</v>
-      </c>
-      <c r="V18" s="67">
-        <v>0</v>
-      </c>
-      <c r="W18" s="67">
-        <v>5</v>
-      </c>
-      <c r="X18" s="66">
+      <c r="S18" s="66">
+        <v>5</v>
+      </c>
+      <c r="T18" s="66">
+        <v>0</v>
+      </c>
+      <c r="U18" s="66">
+        <v>5</v>
+      </c>
+      <c r="V18" s="66">
+        <v>0</v>
+      </c>
+      <c r="W18" s="66">
+        <v>15</v>
+      </c>
+      <c r="X18" s="65">
         <v>2</v>
       </c>
-      <c r="Y18" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AB18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AH18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="67">
-        <v>15</v>
-      </c>
-      <c r="AJ18" s="66">
+      <c r="Y18" s="66">
+        <v>5</v>
+      </c>
+      <c r="Z18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AB18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="67">
+        <v>20</v>
+      </c>
+      <c r="AD18" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AH18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="66">
+        <v>25</v>
+      </c>
+      <c r="AJ18" s="65">
         <v>4</v>
       </c>
-      <c r="AK18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AL18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AN18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AO18" s="68">
-        <v>20</v>
-      </c>
-      <c r="AP18" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AR18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="67">
-        <v>3</v>
-      </c>
-      <c r="AT18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="67">
-        <v>25</v>
+      <c r="AK18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AL18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AN18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="67">
+        <v>30</v>
+      </c>
+      <c r="AP18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AQ18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AR18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="66">
+        <v>5</v>
+      </c>
+      <c r="AT18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="66">
+        <v>35</v>
       </c>
       <c r="AV18" s="38">
         <v>8</v>
       </c>
-      <c r="AW18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AX18" s="67">
-        <v>10</v>
-      </c>
-      <c r="AY18" s="67">
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="67">
+      <c r="AW18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="66">
+        <v>10</v>
+      </c>
+      <c r="AY18" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="66">
         <v>0</v>
       </c>
       <c r="BA18" s="39">
-        <v>40</v>
-      </c>
-      <c r="BB18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BC18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BD18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BE18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF18" s="56">
-        <v>0</v>
-      </c>
-      <c r="BG18" s="56">
-        <v>35</v>
+        <v>60</v>
+      </c>
+      <c r="BB18" s="38">
+        <v>7</v>
+      </c>
+      <c r="BC18" s="66">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="66">
+        <v>10</v>
+      </c>
+      <c r="BE18" s="66">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="66">
+        <v>0</v>
+      </c>
+      <c r="BG18" s="39">
+        <v>80</v>
       </c>
       <c r="BH18" s="55">
         <v>0</v>
@@ -8467,19 +8467,19 @@
       </c>
     </row>
     <row r="19" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63">
+      <c r="A19" s="76">
         <v>17</v>
       </c>
-      <c r="B19" s="64">
-        <v>17</v>
-      </c>
-      <c r="C19" s="65">
-        <v>15</v>
-      </c>
-      <c r="D19" s="66">
-        <v>13</v>
-      </c>
-      <c r="E19" s="67">
+      <c r="B19" s="63">
+        <v>24</v>
+      </c>
+      <c r="C19" s="64">
+        <v>4</v>
+      </c>
+      <c r="D19" s="65">
+        <v>10</v>
+      </c>
+      <c r="E19" s="66">
         <v>28</v>
       </c>
       <c r="F19" s="45">
@@ -8488,11 +8488,11 @@
       <c r="G19" s="45">
         <v>0</v>
       </c>
-      <c r="H19" s="45">
-        <v>0</v>
-      </c>
-      <c r="I19" s="45">
-        <v>0</v>
+      <c r="H19" s="66">
+        <v>10</v>
+      </c>
+      <c r="I19" s="66">
+        <v>20</v>
       </c>
       <c r="J19" s="45">
         <v>0</v>
@@ -8500,131 +8500,131 @@
       <c r="K19" s="43">
         <v>0</v>
       </c>
-      <c r="L19" s="66">
-        <v>0</v>
-      </c>
-      <c r="M19" s="67">
-        <v>3</v>
-      </c>
-      <c r="N19" s="67">
-        <v>0</v>
-      </c>
-      <c r="O19" s="67">
-        <v>0</v>
-      </c>
-      <c r="P19" s="67">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="68">
-        <v>0</v>
-      </c>
-      <c r="R19" s="78">
+      <c r="L19" s="65">
+        <v>0</v>
+      </c>
+      <c r="M19" s="66">
+        <v>0</v>
+      </c>
+      <c r="N19" s="66">
+        <v>0</v>
+      </c>
+      <c r="O19" s="66">
+        <v>10</v>
+      </c>
+      <c r="P19" s="66">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="67">
+        <v>20</v>
+      </c>
+      <c r="R19" s="77">
         <v>1</v>
       </c>
-      <c r="S19" s="67">
-        <v>3</v>
-      </c>
-      <c r="T19" s="67">
-        <v>0</v>
-      </c>
-      <c r="U19" s="67">
-        <v>0</v>
-      </c>
-      <c r="V19" s="67">
-        <v>0</v>
-      </c>
-      <c r="W19" s="67">
-        <v>5</v>
-      </c>
-      <c r="X19" s="66">
+      <c r="S19" s="66">
+        <v>0</v>
+      </c>
+      <c r="T19" s="66">
+        <v>0</v>
+      </c>
+      <c r="U19" s="66">
+        <v>10</v>
+      </c>
+      <c r="V19" s="66">
+        <v>0</v>
+      </c>
+      <c r="W19" s="66">
+        <v>35</v>
+      </c>
+      <c r="X19" s="65">
         <v>2</v>
       </c>
-      <c r="Y19" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD19" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE19" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="67">
-        <v>15</v>
-      </c>
-      <c r="AJ19" s="66">
+      <c r="Y19" s="66">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="66">
+        <v>10</v>
+      </c>
+      <c r="AB19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="67">
+        <v>50</v>
+      </c>
+      <c r="AD19" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="66">
+        <v>10</v>
+      </c>
+      <c r="AH19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="66">
+        <v>65</v>
+      </c>
+      <c r="AJ19" s="65">
         <v>4</v>
       </c>
-      <c r="AK19" s="67">
-        <v>3</v>
-      </c>
-      <c r="AL19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AN19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="68">
-        <v>20</v>
-      </c>
-      <c r="AP19" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ19" s="67">
-        <v>3</v>
-      </c>
-      <c r="AR19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="67">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="67">
-        <v>25</v>
-      </c>
-      <c r="AV19" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW19" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX19" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY19" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA19" s="57">
-        <v>30</v>
+      <c r="AK19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="66">
+        <v>10</v>
+      </c>
+      <c r="AN19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="67">
+        <v>80</v>
+      </c>
+      <c r="AP19" s="66">
+        <v>5</v>
+      </c>
+      <c r="AQ19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="66">
+        <v>10</v>
+      </c>
+      <c r="AT19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="66">
+        <v>95</v>
+      </c>
+      <c r="AV19" s="38">
+        <v>7</v>
+      </c>
+      <c r="AW19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="66">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="66">
+        <v>10</v>
+      </c>
+      <c r="AZ19" s="66">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="39">
+        <v>120</v>
       </c>
       <c r="BB19" s="56">
         <v>0</v>
@@ -8682,19 +8682,19 @@
       </c>
     </row>
     <row r="20" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63">
+      <c r="A20" s="76">
         <v>18</v>
       </c>
-      <c r="B20" s="64">
+      <c r="B20" s="63">
         <v>27</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="64">
         <v>7</v>
       </c>
-      <c r="D20" s="66">
+      <c r="D20" s="65">
         <v>1</v>
       </c>
-      <c r="E20" s="67">
+      <c r="E20" s="66">
         <v>7</v>
       </c>
       <c r="F20" s="45">
@@ -8709,201 +8709,201 @@
       <c r="I20" s="45">
         <v>0</v>
       </c>
-      <c r="J20" s="67">
+      <c r="J20" s="66">
         <v>2</v>
       </c>
-      <c r="K20" s="65">
+      <c r="K20" s="64">
         <v>16</v>
       </c>
-      <c r="L20" s="66">
-        <v>0</v>
-      </c>
-      <c r="M20" s="67">
-        <v>3</v>
-      </c>
-      <c r="N20" s="67">
-        <v>0</v>
-      </c>
-      <c r="O20" s="67">
-        <v>0</v>
-      </c>
-      <c r="P20" s="67">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="68">
-        <v>0</v>
-      </c>
-      <c r="R20" s="78">
-        <v>1</v>
-      </c>
-      <c r="S20" s="67">
-        <v>3</v>
-      </c>
-      <c r="T20" s="67">
-        <v>0</v>
-      </c>
-      <c r="U20" s="67">
-        <v>0</v>
-      </c>
-      <c r="V20" s="67">
-        <v>3</v>
-      </c>
-      <c r="W20" s="67">
-        <v>5</v>
-      </c>
-      <c r="X20" s="66">
-        <v>2</v>
-      </c>
-      <c r="Y20" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AC20" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AH20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AI20" s="67">
-        <v>15</v>
-      </c>
-      <c r="AJ20" s="66">
+      <c r="L20" s="65">
+        <v>3</v>
+      </c>
+      <c r="M20" s="66">
+        <v>10</v>
+      </c>
+      <c r="N20" s="66">
+        <v>0</v>
+      </c>
+      <c r="O20" s="66">
+        <v>0</v>
+      </c>
+      <c r="P20" s="66">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="67">
+        <v>0</v>
+      </c>
+      <c r="R20" s="77">
+        <v>5</v>
+      </c>
+      <c r="S20" s="66">
+        <v>5</v>
+      </c>
+      <c r="T20" s="66">
+        <v>0</v>
+      </c>
+      <c r="U20" s="66">
+        <v>0</v>
+      </c>
+      <c r="V20" s="66">
+        <v>5</v>
+      </c>
+      <c r="W20" s="66">
+        <v>10</v>
+      </c>
+      <c r="X20" s="65">
         <v>4</v>
       </c>
-      <c r="AK20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AL20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AN20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AO20" s="68">
+      <c r="Y20" s="66">
+        <v>5</v>
+      </c>
+      <c r="Z20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="67">
         <v>20</v>
       </c>
-      <c r="AP20" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AR20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="67">
-        <v>3</v>
-      </c>
-      <c r="AU20" s="67">
-        <v>25</v>
-      </c>
-      <c r="AV20" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW20" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY20" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA20" s="57">
+      <c r="AD20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AF20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="66">
         <v>30</v>
       </c>
-      <c r="BB20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BD20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BE20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BG20" s="56">
-        <v>35</v>
-      </c>
-      <c r="BH20" s="55">
-        <v>0</v>
-      </c>
-      <c r="BI20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BJ20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BL20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM20" s="57">
+      <c r="AJ20" s="65">
+        <v>6</v>
+      </c>
+      <c r="AK20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AO20" s="67">
         <v>40</v>
       </c>
-      <c r="BN20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BO20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BP20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BQ20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BR20" s="56">
-        <v>0</v>
-      </c>
-      <c r="BS20" s="58">
-        <v>45</v>
+      <c r="AP20" s="66">
+        <v>4</v>
+      </c>
+      <c r="AQ20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AR20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="66">
+        <v>5</v>
+      </c>
+      <c r="AU20" s="66">
+        <v>50</v>
+      </c>
+      <c r="AV20" s="38">
+        <v>3</v>
+      </c>
+      <c r="AW20" s="66">
+        <v>20</v>
+      </c>
+      <c r="AX20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="66">
+        <v>80</v>
+      </c>
+      <c r="BB20" s="38">
+        <v>3</v>
+      </c>
+      <c r="BC20" s="66">
+        <v>20</v>
+      </c>
+      <c r="BD20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BF20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BG20" s="66">
+        <v>80</v>
+      </c>
+      <c r="BH20" s="38">
+        <v>4</v>
+      </c>
+      <c r="BI20" s="66">
+        <v>20</v>
+      </c>
+      <c r="BJ20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BK20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BM20" s="66">
+        <v>80</v>
+      </c>
+      <c r="BN20" s="38">
+        <v>5</v>
+      </c>
+      <c r="BO20" s="66">
+        <v>20</v>
+      </c>
+      <c r="BP20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BQ20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BR20" s="66">
+        <v>0</v>
+      </c>
+      <c r="BS20" s="100">
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="63">
+      <c r="A21" s="69">
         <v>19</v>
       </c>
-      <c r="B21" s="64">
+      <c r="B21" s="63">
         <v>25</v>
       </c>
-      <c r="C21" s="65">
+      <c r="C21" s="64">
         <v>9</v>
       </c>
       <c r="D21" s="44">
@@ -8924,155 +8924,155 @@
       <c r="I21" s="45">
         <v>0</v>
       </c>
-      <c r="J21" s="67">
+      <c r="J21" s="66">
         <v>2</v>
       </c>
-      <c r="K21" s="65">
+      <c r="K21" s="64">
         <v>16</v>
       </c>
-      <c r="L21" s="66">
-        <v>0</v>
-      </c>
-      <c r="M21" s="67">
-        <v>0</v>
-      </c>
-      <c r="N21" s="67">
-        <v>0</v>
-      </c>
-      <c r="O21" s="67">
-        <v>0</v>
-      </c>
-      <c r="P21" s="67">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="68">
-        <v>0</v>
-      </c>
-      <c r="R21" s="78">
+      <c r="L21" s="65">
+        <v>0</v>
+      </c>
+      <c r="M21" s="66">
+        <v>0</v>
+      </c>
+      <c r="N21" s="66">
+        <v>0</v>
+      </c>
+      <c r="O21" s="66">
+        <v>0</v>
+      </c>
+      <c r="P21" s="66">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="67">
+        <v>0</v>
+      </c>
+      <c r="R21" s="77">
         <v>1</v>
       </c>
-      <c r="S21" s="67">
-        <v>0</v>
-      </c>
-      <c r="T21" s="67">
-        <v>0</v>
-      </c>
-      <c r="U21" s="67">
-        <v>0</v>
-      </c>
-      <c r="V21" s="67">
-        <v>3</v>
-      </c>
-      <c r="W21" s="67">
-        <v>5</v>
-      </c>
-      <c r="X21" s="66">
+      <c r="S21" s="66">
+        <v>0</v>
+      </c>
+      <c r="T21" s="66">
+        <v>0</v>
+      </c>
+      <c r="U21" s="66">
+        <v>0</v>
+      </c>
+      <c r="V21" s="66">
+        <v>10</v>
+      </c>
+      <c r="W21" s="66">
+        <v>5</v>
+      </c>
+      <c r="X21" s="65">
         <v>2</v>
       </c>
-      <c r="Y21" s="67">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="67">
-        <v>3</v>
-      </c>
-      <c r="AC21" s="68">
-        <v>10</v>
-      </c>
-      <c r="AD21" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AH21" s="67">
-        <v>3</v>
-      </c>
-      <c r="AI21" s="67">
+      <c r="Y21" s="66">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="66">
+        <v>10</v>
+      </c>
+      <c r="AC21" s="67">
+        <v>10</v>
+      </c>
+      <c r="AD21" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="66">
+        <v>10</v>
+      </c>
+      <c r="AI21" s="66">
         <v>15</v>
       </c>
-      <c r="AJ21" s="66">
+      <c r="AJ21" s="65">
         <v>4</v>
       </c>
-      <c r="AK21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AL21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AN21" s="67">
-        <v>3</v>
-      </c>
-      <c r="AO21" s="68">
+      <c r="AK21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="66">
+        <v>10</v>
+      </c>
+      <c r="AO21" s="67">
         <v>20</v>
       </c>
-      <c r="AP21" s="67">
-        <v>5</v>
-      </c>
-      <c r="AQ21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AR21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AS21" s="67">
-        <v>0</v>
-      </c>
-      <c r="AT21" s="67">
-        <v>3</v>
-      </c>
-      <c r="AU21" s="67">
+      <c r="AP21" s="66">
+        <v>5</v>
+      </c>
+      <c r="AQ21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="66">
+        <v>10</v>
+      </c>
+      <c r="AU21" s="66">
         <v>25</v>
       </c>
-      <c r="AV21" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW21" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX21" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY21" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA21" s="57">
-        <v>30</v>
-      </c>
-      <c r="BB21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BD21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BE21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF21" s="56">
-        <v>0</v>
-      </c>
-      <c r="BG21" s="56">
-        <v>35</v>
+      <c r="AV21" s="38">
+        <v>7</v>
+      </c>
+      <c r="AW21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="66">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="66">
+        <v>5</v>
+      </c>
+      <c r="BA21" s="66">
+        <v>40</v>
+      </c>
+      <c r="BB21" s="38">
+        <v>8</v>
+      </c>
+      <c r="BC21" s="66">
+        <v>0</v>
+      </c>
+      <c r="BD21" s="66">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="66">
+        <v>0</v>
+      </c>
+      <c r="BF21" s="66">
+        <v>5</v>
+      </c>
+      <c r="BG21" s="66">
+        <v>40</v>
       </c>
       <c r="BH21" s="55">
         <v>0</v>
@@ -15703,86 +15703,81 @@
       <c r="AU52" s="52">
         <v>25</v>
       </c>
-      <c r="AV52" s="73">
-        <v>0</v>
-      </c>
-      <c r="AW52" s="74">
-        <v>0</v>
-      </c>
-      <c r="AX52" s="74">
-        <v>0</v>
-      </c>
-      <c r="AY52" s="74">
-        <v>0</v>
-      </c>
-      <c r="AZ52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BA52" s="75">
+      <c r="AV52" s="72">
+        <v>0</v>
+      </c>
+      <c r="AW52" s="73">
+        <v>0</v>
+      </c>
+      <c r="AX52" s="73">
+        <v>0</v>
+      </c>
+      <c r="AY52" s="73">
+        <v>0</v>
+      </c>
+      <c r="AZ52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BA52" s="74">
         <v>30</v>
       </c>
-      <c r="BB52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BC52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BD52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BE52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BF52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BG52" s="74">
+      <c r="BB52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BC52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BD52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BE52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BF52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BG52" s="73">
         <v>35</v>
       </c>
-      <c r="BH52" s="73">
-        <v>0</v>
-      </c>
-      <c r="BI52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BJ52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BK52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BL52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BM52" s="75">
+      <c r="BH52" s="72">
+        <v>0</v>
+      </c>
+      <c r="BI52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BJ52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BK52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BL52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BM52" s="74">
         <v>40</v>
       </c>
-      <c r="BN52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BO52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BP52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BQ52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BR52" s="74">
-        <v>0</v>
-      </c>
-      <c r="BS52" s="76">
+      <c r="BN52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BO52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BP52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BQ52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BR52" s="73">
+        <v>0</v>
+      </c>
+      <c r="BS52" s="75">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
@@ -15795,6 +15790,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Modif select & target TOWER
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1321,10 +1321,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1336,34 +1354,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1376,9 +1379,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="87" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2609,7 +2609,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2635,10 +2635,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2663,8 +2663,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
-      <c r="B5" s="82"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2687,8 +2687,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="90"/>
+      <c r="B6" s="88" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2713,8 +2713,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="82"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2737,8 +2737,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="82" t="s">
+      <c r="A8" s="90"/>
+      <c r="B8" s="88" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2763,8 +2763,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="82"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2787,8 +2787,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="84"/>
-      <c r="B10" s="82" t="s">
+      <c r="A10" s="90"/>
+      <c r="B10" s="88" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2813,8 +2813,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="83"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2837,7 +2837,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="80" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2995,7 +2995,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="80" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3179,7 +3179,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
+      <c r="A25" s="82"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="80" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3363,7 +3363,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
+      <c r="A32" s="82"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="80" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3547,7 +3547,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="88"/>
+      <c r="A39" s="82"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="80" t="s">
+      <c r="A40" s="83" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3757,7 +3757,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="80" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3915,7 +3915,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="88"/>
+      <c r="A53" s="82"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3941,7 +3941,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="83" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4125,7 +4125,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="87" t="s">
+      <c r="A61" s="80" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4283,7 +4283,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="88"/>
+      <c r="A67" s="82"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4309,7 +4309,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="87" t="s">
+      <c r="A68" s="80" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4467,7 +4467,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="88"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4493,7 +4493,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="80" t="s">
+      <c r="A75" s="83" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4651,7 +4651,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="90"/>
+      <c r="A81" s="84"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4678,23 +4678,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4709,7 +4709,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BN20" sqref="BN20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4720,128 +4720,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="98" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="94" t="s">
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="93" t="s">
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-      <c r="X1" s="94" t="s">
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="94"/>
-      <c r="Z1" s="94"/>
-      <c r="AA1" s="94"/>
-      <c r="AB1" s="94"/>
-      <c r="AC1" s="94"/>
-      <c r="AD1" s="93" t="s">
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93"/>
-      <c r="AJ1" s="94" t="s">
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="94"/>
-      <c r="AL1" s="94"/>
-      <c r="AM1" s="94"/>
-      <c r="AN1" s="94"/>
-      <c r="AO1" s="94"/>
-      <c r="AP1" s="93" t="s">
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" s="93"/>
-      <c r="AR1" s="93"/>
-      <c r="AS1" s="93"/>
-      <c r="AT1" s="93"/>
-      <c r="AU1" s="93"/>
-      <c r="AV1" s="94" t="s">
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="AW1" s="94"/>
-      <c r="AX1" s="94"/>
-      <c r="AY1" s="94"/>
-      <c r="AZ1" s="94"/>
-      <c r="BA1" s="94"/>
-      <c r="BB1" s="93" t="s">
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="91"/>
+      <c r="AY1" s="91"/>
+      <c r="AZ1" s="91"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="BC1" s="93"/>
-      <c r="BD1" s="93"/>
-      <c r="BE1" s="93"/>
-      <c r="BF1" s="93"/>
-      <c r="BG1" s="93"/>
-      <c r="BH1" s="94" t="s">
+      <c r="BC1" s="92"/>
+      <c r="BD1" s="92"/>
+      <c r="BE1" s="92"/>
+      <c r="BF1" s="92"/>
+      <c r="BG1" s="92"/>
+      <c r="BH1" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="94"/>
-      <c r="BJ1" s="94"/>
-      <c r="BK1" s="94"/>
-      <c r="BL1" s="94"/>
-      <c r="BM1" s="94"/>
-      <c r="BN1" s="93" t="s">
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="91"/>
+      <c r="BK1" s="91"/>
+      <c r="BL1" s="91"/>
+      <c r="BM1" s="91"/>
+      <c r="BN1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="BO1" s="93"/>
-      <c r="BP1" s="93"/>
-      <c r="BQ1" s="93"/>
-      <c r="BR1" s="93"/>
-      <c r="BS1" s="99"/>
+      <c r="BO1" s="92"/>
+      <c r="BP1" s="92"/>
+      <c r="BQ1" s="92"/>
+      <c r="BR1" s="92"/>
+      <c r="BS1" s="93"/>
     </row>
     <row r="2" spans="1:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92"/>
+      <c r="A2" s="95"/>
       <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="97" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97" t="s">
+      <c r="D2" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97" t="s">
+      <c r="G2" s="98"/>
+      <c r="H2" s="98" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="97"/>
+      <c r="K2" s="98"/>
       <c r="L2" s="26" t="s">
         <v>28</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="34">
         <v>9</v>
@@ -15775,6 +15775,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L1:Q1"/>
     <mergeCell ref="AV1:BA1"/>
     <mergeCell ref="BB1:BG1"/>
     <mergeCell ref="BH1:BM1"/>
@@ -15791,7 +15792,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
-    <mergeCell ref="L1:Q1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Tunning select & target TOWER
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1321,28 +1321,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1352,6 +1334,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2609,7 +2609,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="87"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2635,10 +2635,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="82" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2663,8 +2663,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="88"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2687,8 +2687,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="90"/>
-      <c r="B6" s="88" t="s">
+      <c r="A6" s="84"/>
+      <c r="B6" s="82" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2713,8 +2713,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="88"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2737,8 +2737,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="90"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="82" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2763,8 +2763,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2787,8 +2787,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="90"/>
-      <c r="B10" s="88" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="82" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2813,8 +2813,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="90"/>
-      <c r="B11" s="89"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2837,7 +2837,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="87" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2995,7 +2995,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="82"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="87" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3179,7 +3179,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
+      <c r="A25" s="88"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="87" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3363,7 +3363,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="82"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="87" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3547,7 +3547,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="82"/>
+      <c r="A39" s="88"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="83" t="s">
+      <c r="A40" s="80" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3757,7 +3757,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="80" t="s">
+      <c r="A47" s="87" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3915,7 +3915,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="82"/>
+      <c r="A53" s="88"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3941,7 +3941,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="83" t="s">
+      <c r="A54" s="80" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4125,7 +4125,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="80" t="s">
+      <c r="A61" s="87" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4283,7 +4283,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="82"/>
+      <c r="A67" s="88"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4309,7 +4309,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="80" t="s">
+      <c r="A68" s="87" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4467,7 +4467,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="82"/>
+      <c r="A74" s="88"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4493,7 +4493,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="83" t="s">
+      <c r="A75" s="80" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4651,7 +4651,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="84"/>
+      <c r="A81" s="90"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4678,23 +4678,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4709,7 +4709,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5023,7 +5023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="68">
         <v>1</v>
       </c>
@@ -5238,218 +5238,218 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69">
+    <row r="4" spans="1:71" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68">
         <v>2</v>
       </c>
-      <c r="B4" s="32">
-        <v>3</v>
-      </c>
-      <c r="C4" s="34">
+      <c r="B4" s="31">
+        <v>2</v>
+      </c>
+      <c r="C4" s="33">
         <v>9</v>
       </c>
-      <c r="D4" s="38">
-        <v>7</v>
-      </c>
-      <c r="E4" s="30">
-        <v>28</v>
-      </c>
-      <c r="F4" s="30">
+      <c r="D4" s="62">
+        <v>0</v>
+      </c>
+      <c r="E4" s="60">
+        <v>0</v>
+      </c>
+      <c r="F4" s="28">
         <v>2</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="28">
+        <v>16</v>
+      </c>
+      <c r="H4" s="60">
+        <v>0</v>
+      </c>
+      <c r="I4" s="60">
+        <v>0</v>
+      </c>
+      <c r="J4" s="60">
+        <v>0</v>
+      </c>
+      <c r="K4" s="61">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36">
+        <v>0</v>
+      </c>
+      <c r="M4" s="28">
+        <v>0</v>
+      </c>
+      <c r="N4" s="28">
+        <v>10</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0</v>
+      </c>
+      <c r="P4" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="37">
+        <v>5</v>
+      </c>
+      <c r="R4" s="36">
+        <v>0</v>
+      </c>
+      <c r="S4" s="28">
+        <v>0</v>
+      </c>
+      <c r="T4" s="28">
+        <v>10</v>
+      </c>
+      <c r="U4" s="28">
+        <v>0</v>
+      </c>
+      <c r="V4" s="28">
+        <v>0</v>
+      </c>
+      <c r="W4" s="37">
+        <v>10</v>
+      </c>
+      <c r="X4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="28">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="37">
         <v>15</v>
       </c>
-      <c r="H4" s="30">
-        <v>7</v>
-      </c>
-      <c r="I4" s="30">
-        <v>28</v>
-      </c>
-      <c r="J4" s="30">
-        <v>4</v>
-      </c>
-      <c r="K4" s="34">
-        <v>14</v>
-      </c>
-      <c r="L4" s="38">
-        <v>0</v>
-      </c>
-      <c r="M4" s="30">
-        <v>0</v>
-      </c>
-      <c r="N4" s="30">
-        <v>10</v>
-      </c>
-      <c r="O4" s="30">
-        <v>0</v>
-      </c>
-      <c r="P4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="39">
-        <v>5</v>
-      </c>
-      <c r="R4" s="35">
-        <v>0</v>
-      </c>
-      <c r="S4" s="30">
-        <v>0</v>
-      </c>
-      <c r="T4" s="30">
-        <v>0</v>
-      </c>
-      <c r="U4" s="30">
-        <v>10</v>
-      </c>
-      <c r="V4" s="30">
-        <v>0</v>
-      </c>
-      <c r="W4" s="30">
-        <v>10</v>
-      </c>
-      <c r="X4" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="30">
-        <v>10</v>
-      </c>
-      <c r="Z4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="39">
+      <c r="AD4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="28">
+        <v>10</v>
+      </c>
+      <c r="AG4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="37">
         <v>15</v>
       </c>
-      <c r="AD4" s="30">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="30">
-        <v>5</v>
-      </c>
-      <c r="AG4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="30">
+      <c r="AJ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="28">
+        <v>10</v>
+      </c>
+      <c r="AM4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="37">
+        <v>20</v>
+      </c>
+      <c r="AP4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="28">
+        <v>10</v>
+      </c>
+      <c r="AS4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="37">
+        <v>25</v>
+      </c>
+      <c r="AV4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="28">
+        <v>10</v>
+      </c>
+      <c r="AY4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="37">
         <v>30</v>
       </c>
-      <c r="AJ4" s="38">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="30">
-        <v>5</v>
-      </c>
-      <c r="AM4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="39">
+      <c r="BB4" s="36">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="28">
+        <v>10</v>
+      </c>
+      <c r="BE4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="37">
         <v>35</v>
       </c>
-      <c r="AP4" s="30">
-        <v>2</v>
-      </c>
-      <c r="AQ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AS4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="30">
-        <v>45</v>
-      </c>
-      <c r="AV4" s="55">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="56">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="56">
-        <v>0</v>
-      </c>
-      <c r="AY4" s="56">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BA4" s="57">
-        <v>60</v>
-      </c>
-      <c r="BB4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BD4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BG4" s="56">
-        <v>60</v>
-      </c>
-      <c r="BH4" s="55">
-        <v>0</v>
-      </c>
-      <c r="BI4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="57">
+      <c r="BH4" s="36">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="28">
+        <v>10</v>
+      </c>
+      <c r="BK4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="37">
         <v>40</v>
       </c>
-      <c r="BN4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="56">
-        <v>0</v>
-      </c>
-      <c r="BS4" s="58">
+      <c r="BN4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="28">
+        <v>10</v>
+      </c>
+      <c r="BQ4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="28">
+        <v>0</v>
+      </c>
+      <c r="BS4" s="29">
         <v>45</v>
       </c>
     </row>
@@ -9109,146 +9109,146 @@
       </c>
     </row>
     <row r="22" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41">
+      <c r="A22" s="69">
         <v>20</v>
       </c>
-      <c r="B22" s="42">
-        <v>10</v>
-      </c>
-      <c r="C22" s="43">
-        <v>10</v>
-      </c>
-      <c r="D22" s="44">
-        <v>5</v>
-      </c>
-      <c r="E22" s="45">
-        <v>25</v>
-      </c>
-      <c r="F22" s="45">
+      <c r="B22" s="32">
+        <v>3</v>
+      </c>
+      <c r="C22" s="34">
+        <v>9</v>
+      </c>
+      <c r="D22" s="38">
+        <v>7</v>
+      </c>
+      <c r="E22" s="30">
+        <v>28</v>
+      </c>
+      <c r="F22" s="30">
+        <v>2</v>
+      </c>
+      <c r="G22" s="30">
+        <v>15</v>
+      </c>
+      <c r="H22" s="30">
+        <v>7</v>
+      </c>
+      <c r="I22" s="30">
+        <v>28</v>
+      </c>
+      <c r="J22" s="30">
         <v>4</v>
       </c>
-      <c r="G22" s="45">
+      <c r="K22" s="34">
         <v>14</v>
       </c>
-      <c r="H22" s="45">
-        <v>5</v>
-      </c>
-      <c r="I22" s="45">
-        <v>25</v>
-      </c>
-      <c r="J22" s="45">
-        <v>4</v>
-      </c>
-      <c r="K22" s="43">
-        <v>14</v>
-      </c>
-      <c r="L22" s="44">
-        <v>0</v>
-      </c>
-      <c r="M22" s="45">
-        <v>0</v>
-      </c>
-      <c r="N22" s="45">
-        <v>0</v>
-      </c>
-      <c r="O22" s="45">
-        <v>0</v>
-      </c>
-      <c r="P22" s="45">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="46">
-        <v>0</v>
-      </c>
-      <c r="R22" s="47">
+      <c r="L22" s="38">
+        <v>0</v>
+      </c>
+      <c r="M22" s="30">
+        <v>0</v>
+      </c>
+      <c r="N22" s="30">
+        <v>10</v>
+      </c>
+      <c r="O22" s="30">
+        <v>0</v>
+      </c>
+      <c r="P22" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="39">
+        <v>5</v>
+      </c>
+      <c r="R22" s="35">
+        <v>0</v>
+      </c>
+      <c r="S22" s="30">
+        <v>0</v>
+      </c>
+      <c r="T22" s="30">
+        <v>0</v>
+      </c>
+      <c r="U22" s="30">
+        <v>10</v>
+      </c>
+      <c r="V22" s="30">
+        <v>0</v>
+      </c>
+      <c r="W22" s="30">
+        <v>10</v>
+      </c>
+      <c r="X22" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="30">
+        <v>10</v>
+      </c>
+      <c r="Z22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="39">
+        <v>15</v>
+      </c>
+      <c r="AD22" s="30">
         <v>1</v>
       </c>
-      <c r="S22" s="45">
-        <v>0</v>
-      </c>
-      <c r="T22" s="45">
-        <v>0</v>
-      </c>
-      <c r="U22" s="45">
-        <v>0</v>
-      </c>
-      <c r="V22" s="45">
-        <v>3</v>
-      </c>
-      <c r="W22" s="45">
-        <v>5</v>
-      </c>
-      <c r="X22" s="44">
+      <c r="AE22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="30">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="30">
+        <v>30</v>
+      </c>
+      <c r="AJ22" s="38">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="30">
+        <v>5</v>
+      </c>
+      <c r="AM22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO22" s="39">
+        <v>35</v>
+      </c>
+      <c r="AP22" s="30">
         <v>2</v>
       </c>
-      <c r="Y22" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="45">
-        <v>3</v>
-      </c>
-      <c r="AC22" s="46">
-        <v>10</v>
-      </c>
-      <c r="AD22" s="45">
-        <v>3</v>
-      </c>
-      <c r="AE22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="45">
-        <v>3</v>
-      </c>
-      <c r="AI22" s="45">
-        <v>15</v>
-      </c>
-      <c r="AJ22" s="44">
-        <v>4</v>
-      </c>
-      <c r="AK22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN22" s="45">
-        <v>3</v>
-      </c>
-      <c r="AO22" s="46">
-        <v>20</v>
-      </c>
-      <c r="AP22" s="45">
-        <v>5</v>
-      </c>
-      <c r="AQ22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT22" s="45">
-        <v>3</v>
-      </c>
-      <c r="AU22" s="45">
-        <v>25</v>
+      <c r="AQ22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="30">
+        <v>10</v>
+      </c>
+      <c r="AS22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="30">
+        <v>45</v>
       </c>
       <c r="AV22" s="55">
         <v>0</v>
@@ -9266,7 +9266,7 @@
         <v>0</v>
       </c>
       <c r="BA22" s="57">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="BB22" s="56">
         <v>0</v>
@@ -9284,7 +9284,7 @@
         <v>0</v>
       </c>
       <c r="BG22" s="56">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="BH22" s="55">
         <v>0</v>
@@ -15775,11 +15775,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
@@ -15792,6 +15787,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Correct Bug Level 16
</commit_message>
<xml_diff>
--- a/DOC/BoatsAttackGame.xlsx
+++ b/DOC/BoatsAttackGame.xlsx
@@ -1310,10 +1310,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1323,24 +1341,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="88" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2598,7 +2598,7 @@
       <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2624,10 +2624,10 @@
       <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="89" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12"/>
@@ -2652,8 +2652,8 @@
       <c r="V4" s="14"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2676,8 +2676,8 @@
       <c r="V5" s="14"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="91"/>
+      <c r="B6" s="89" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="12"/>
@@ -2702,8 +2702,8 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="85"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="89"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2726,8 +2726,8 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
-      <c r="B8" s="83" t="s">
+      <c r="A8" s="91"/>
+      <c r="B8" s="89" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12"/>
@@ -2752,8 +2752,8 @@
       <c r="V8" s="14"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2776,8 +2776,8 @@
       <c r="V9" s="14"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
-      <c r="B10" s="83" t="s">
+      <c r="A10" s="91"/>
+      <c r="B10" s="89" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
@@ -2802,8 +2802,8 @@
       <c r="V10" s="14"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2826,7 +2826,7 @@
       <c r="V11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="81" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -2984,7 +2984,7 @@
       <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="23" t="s">
         <v>17</v>
       </c>
@@ -3010,7 +3010,7 @@
       <c r="V18" s="17"/>
     </row>
     <row r="19" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="81" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3168,7 +3168,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="23" t="s">
         <v>17</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="V25" s="17"/>
     </row>
     <row r="26" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="81" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3352,7 +3352,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="23" t="s">
         <v>17</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="V32" s="17"/>
     </row>
     <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="81" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3536,7 +3536,7 @@
       <c r="V38" s="14"/>
     </row>
     <row r="39" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="23" t="s">
         <v>17</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="V39" s="17"/>
     </row>
     <row r="40" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="84" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -3746,7 +3746,7 @@
       <c r="V46" s="17"/>
     </row>
     <row r="47" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="81" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="18" t="s">
@@ -3904,7 +3904,7 @@
       <c r="V52" s="14"/>
     </row>
     <row r="53" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="89"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="23" t="s">
         <v>17</v>
       </c>
@@ -3930,7 +3930,7 @@
       <c r="V53" s="17"/>
     </row>
     <row r="54" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="84" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="18" t="s">
@@ -4114,7 +4114,7 @@
       <c r="V60" s="17"/>
     </row>
     <row r="61" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88" t="s">
+      <c r="A61" s="81" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -4272,7 +4272,7 @@
       <c r="V66" s="14"/>
     </row>
     <row r="67" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="89"/>
+      <c r="A67" s="83"/>
       <c r="B67" s="23" t="s">
         <v>17</v>
       </c>
@@ -4298,7 +4298,7 @@
       <c r="V67" s="17"/>
     </row>
     <row r="68" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="81" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -4456,7 +4456,7 @@
       <c r="V73" s="14"/>
     </row>
     <row r="74" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="89"/>
+      <c r="A74" s="83"/>
       <c r="B74" s="23" t="s">
         <v>17</v>
       </c>
@@ -4482,7 +4482,7 @@
       <c r="V74" s="17"/>
     </row>
     <row r="75" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="81" t="s">
+      <c r="A75" s="84" t="s">
         <v>26</v>
       </c>
       <c r="B75" s="18" t="s">
@@ -4640,7 +4640,7 @@
       <c r="V80" s="14"/>
     </row>
     <row r="81" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="91"/>
+      <c r="A81" s="85"/>
       <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
@@ -4667,23 +4667,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A75:A81"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4698,7 +4698,7 @@
   <dimension ref="A1:BS52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8257,7 +8257,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="57">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="57">
         <v>1</v>
@@ -15764,11 +15764,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="BN1:BS1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
@@ -15781,6 +15776,11 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="BN1:BS1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>